<commit_message>
students excel file and StudentReader added
</commit_message>
<xml_diff>
--- a/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
+++ b/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="236">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,28 +26,490 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Ringo Starr</t>
-  </si>
-  <si>
-    <t>The Beatles and the Cthulu mythos</t>
+    <t>Lara Croft</t>
+  </si>
+  <si>
+    <t>Tomb Raider and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>looking for hidden treasures in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>unearthing ancient tombs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Fred Astaire</t>
+  </si>
+  <si>
+    <t>Dancing and the Cthulu mythos</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
-    <t xml:space="preserve"> Pop music and the Cthulu mythos</t>
+    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in romantic comedies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dexter Morgan</t>
+  </si>
+  <si>
+    <t>Miami-Dade and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>chasing murderers in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> killing murderers in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dave Lee Roth</t>
+  </si>
+  <si>
+    <t>Rock music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Enrico Caruso</t>
+  </si>
+  <si>
+    <t>Opera and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>singing opera arias in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Janis Joplin</t>
+  </si>
+  <si>
+    <t>Psychadelic music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Tony Stark</t>
+  </si>
+  <si>
+    <t>Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Technology and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a multinational corporation in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Pablo Escobar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> International Crime and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a criminal enterprise in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> running a crime family in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Barney Gumble</t>
+  </si>
+  <si>
+    <t>The Simpsons and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>drinking one's life away in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Mike  Pence</t>
+  </si>
+  <si>
+    <t>the Right and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Republicans and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Coco Chanel</t>
+  </si>
+  <si>
+    <t>Fashion and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Rag Trade and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Fashion industry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Edith Piaf</t>
+  </si>
+  <si>
+    <t>Cabaret singing and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing melancholy songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Kylie Minogue</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu mythos</t>
   </si>
   <si>
     <t>singing pop songs in Cthulhu-worshipping societies</t>
   </si>
   <si>
-    <t>Inspector Endeavour Morse</t>
-  </si>
-  <si>
-    <t>Oxford and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>DS</t>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Pythagoras</t>
+  </si>
+  <si>
+    <t>Mathematics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ancient Greece and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>studying mathematics in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ilya Kuryakin</t>
+  </si>
+  <si>
+    <t>The Man from U.N.C.L.E and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Hillary Clinton</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Left and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Democrats and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Willie Nelson</t>
+  </si>
+  <si>
+    <t>Country music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing country music in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Waylon Smithers</t>
+  </si>
+  <si>
+    <t>Nuclear Power and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Simpsons and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>fawning on the boss in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Thomas Edison</t>
+  </si>
+  <si>
+    <t>Physics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electricity and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>pioneering new technologies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>LeBron James</t>
+  </si>
+  <si>
+    <t>Basketball and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>playing basketball in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making dunk shots in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Princess Leia Organa</t>
+  </si>
+  <si>
+    <t>Star Wars and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>leading the rebel alliance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> smuggling military plans in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Pocahontas</t>
+  </si>
+  <si>
+    <t>American history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the New world and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>bridging cultures  in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>G. Gordon Liddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ranting about liberals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bugging political rivals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pulling dirty political tricks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Professor Hans Zarkov</t>
+  </si>
+  <si>
+    <t>Flash Gordon and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>building rocket ships in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Doc Emmett Brown</t>
+  </si>
+  <si>
+    <t>Back To The Future and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>pioneering new technologies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> developing new technologies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>William Randolph Hearst</t>
+  </si>
+  <si>
+    <t>the Newspaper industry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a media empire in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> publishing newspapers in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Larry Flynt</t>
+  </si>
+  <si>
+    <t>Hustler Magazine and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soft pornography and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>publishing soft pornography in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Samwise Gamgee</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hobbit and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>tending the garden in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Babe Ruth</t>
+  </si>
+  <si>
+    <t>Baseball and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American sports and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>hitting home runs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Polonius</t>
+  </si>
+  <si>
+    <t>Denmark and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Elsinore and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hamlet: Prince of Denmark and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Selma Bouvier</t>
+  </si>
+  <si>
+    <t>smoking Laramie Hi-Tars in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> watching MacGyver reruns in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> clipping coupons in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jim Carrey</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>gurning for the camera in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Savonarola</t>
+  </si>
+  <si>
+    <t>Florence and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Renaissance and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting conservative values in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Kenny G</t>
+  </si>
+  <si>
+    <t>Easy Listening and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Light Jazz and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Saxophone music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Deep Throat</t>
+  </si>
+  <si>
+    <t>Watergate and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>talking in riddles in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> offering advice in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Keyser Söze</t>
+  </si>
+  <si>
+    <t>The Usual Suspects and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a criminal enterprise in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eluding the FBI in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Reince Priebus</t>
+  </si>
+  <si>
+    <t>the Right and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Jimi Hendrix</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Guitar music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> playing rock guitar in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Uriah Heap</t>
+  </si>
+  <si>
+    <t>David Copperfield and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Bette Midler</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing torch songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> over-acting in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Daniel Craig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> James Bond and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in action movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in indy movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Philip Marlowe</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Dagon mythos</t>
   </si>
   <si>
     <t>solving mysteries in Dagon-worshipping societies</t>
@@ -56,664 +518,208 @@
     <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
   </si>
   <si>
-    <t>Sam Winchester</t>
+    <t>Judge Joe Dredd</t>
+  </si>
+  <si>
+    <t>Mega-City One and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>tracking down criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> preventing crime in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern science and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Cosmos and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting science in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Indiana Jones</t>
+  </si>
+  <si>
+    <t>Raiders of the Lost Ark and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Archeology and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> punching out Nazis in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Captain Ahab</t>
+  </si>
+  <si>
+    <t>Moby Dick and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Whaling and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>chasing a great white whale in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Monsieur Hulot</t>
+  </si>
+  <si>
+    <t>French comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> French humour and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>causing mayhem in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Helen Keller</t>
+  </si>
+  <si>
+    <t>American education and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>reading braille in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avoiding eye contact in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Rico Tubbs</t>
+  </si>
+  <si>
+    <t>Miami Vice and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arresting drug dealers in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>David Lynch</t>
+  </si>
+  <si>
+    <t>Movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Twin Peaks and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>directing weird movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dorian Gray</t>
+  </si>
+  <si>
+    <t>The Picture of Dorian Gray and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>gadding about town in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> practicing good skin care in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>John Calvin</t>
+  </si>
+  <si>
+    <t>Religious Iconology and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Hans Gruber</t>
+  </si>
+  <si>
+    <t>Die Hard and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Nakatomi building and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>organizing armed robberies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Buffy Summers</t>
   </si>
   <si>
     <t>Horror and the Dagon mythos</t>
   </si>
   <si>
-    <t xml:space="preserve"> Supernatural and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Demonology and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Barney Rubble</t>
-  </si>
-  <si>
-    <t>Bedrock and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Neolithic times and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>pedalling engine-less cars in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Donald Duck</t>
-  </si>
-  <si>
-    <t>Walt Disney animation and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>eating Peking duck in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> setting mousetraps in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Woody Allen</t>
-  </si>
-  <si>
-    <t>New York City and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Frank Capra</t>
-  </si>
-  <si>
-    <t>It's a Wonderful Life and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>making idealistic movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joseph McCarthy</t>
-  </si>
-  <si>
-    <t>American history and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for democracy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jenna Maroney</t>
-  </si>
-  <si>
-    <t>30 Rock and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Television Production and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joseph Goebbels</t>
-  </si>
-  <si>
-    <t>the Nazi Party and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> National Socialism and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Third Reich and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Walt Longmire</t>
-  </si>
-  <si>
-    <t>Crime fiction and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Detective fiction and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>solving mysteries in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Forrest Gump</t>
-  </si>
-  <si>
-    <t>Greenbow Alabama and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the American South and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fishing for shrimps in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pete Sampras</t>
-  </si>
-  <si>
-    <t>Tennis and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>winning tennis matches in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> winning tennis grand slams in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Charlie Brown</t>
-  </si>
-  <si>
-    <t>Peanuts and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American culture and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>playing baseball in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Thomas Jefferson</t>
-  </si>
-  <si>
-    <t>American history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>campaigning for democracy in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Amelia Earhart</t>
-  </si>
-  <si>
-    <t>Aviation and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American history and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>flying airplanes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Kevin Spacey</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Juliet Capulet</t>
-  </si>
-  <si>
-    <t>Romeo and Juliet and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>watching the sun rise in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ashton Kutcher</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in sit-coms in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Patch Adams</t>
-  </si>
-  <si>
-    <t>Modern medicine and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>treating the sick with jokes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making sick people laugh in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joan Crawford</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Christina Aguilera</t>
-  </si>
-  <si>
-    <t>Pop Music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Walter Mitty</t>
-  </si>
-  <si>
-    <t>Escapism and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>dreaming the day away in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> escaping from reality in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mike  Pence</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ned Flanders</t>
-  </si>
-  <si>
-    <t>The Simpsons and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tina Turner</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Letterman</t>
-  </si>
-  <si>
-    <t>Late-night TV and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chat Shows and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CBS and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Ali G</t>
-  </si>
-  <si>
-    <t>Ali G Indahouse and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>interviewing celebrities in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joe Biden</t>
-  </si>
-  <si>
-    <t>the Left and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Democrats and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>plagiarizing political speeches in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Hillary Clinton</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Left and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running for the senate in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Glenn Quagmire</t>
-  </si>
-  <si>
-    <t>Family Guy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>chasing women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> exploiting women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Svengali</t>
-  </si>
-  <si>
-    <t>the Music industry and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>manipulating ingenues in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Huckleberry Finn</t>
-  </si>
-  <si>
-    <t>American literature and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>growing up poor in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Seth MacFarlane</t>
-  </si>
-  <si>
-    <t>Family Guy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>making vulgar jokes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making vulgar cartoons in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Yoda</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for the resistance in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> promoting mysticism in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>The Joker</t>
+    <t>hunting demons in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hunting monsters in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stanley Kowalski</t>
+  </si>
+  <si>
+    <t>A Street Car Named Desire and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>moaning about women in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Lee Marvin</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> War movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Shylock</t>
+  </si>
+  <si>
+    <t>Shakespeare and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>amassing wealth in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> seeking revenge in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Roseanne Barr</t>
+  </si>
+  <si>
+    <t>Televison and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making vulgar jokes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Santa Claus</t>
+  </si>
+  <si>
+    <t>the North Pole and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christmas and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>delivering presents in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>General Zod</t>
   </si>
   <si>
     <t>DC Comics and the Dagon mythos</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gotham City and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>causing mayhem in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Dr. Julius No</t>
-  </si>
-  <si>
-    <t>James Bond and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Terrorism and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Finance and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Bill Gates</t>
-  </si>
-  <si>
-    <t>Microsoft and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Technology and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Software and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Oliver Cromwell</t>
-  </si>
-  <si>
-    <t>British history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British royalty and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fighting with swords in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Le Chiffre</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cheating at poker in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> playing Baccarat  in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Robert Mueller</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Law and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>chasing criminals in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> interviewing politicians in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Linus Torvalds</t>
-  </si>
-  <si>
-    <t>Linux and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Operating Systems and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>developing open-source software in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joaquin Phoenix</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Serious Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in action movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in indy movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>P. T. Barnum</t>
-  </si>
-  <si>
-    <t>the Circus and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Showmanship and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting circus attractions in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bridget Jones</t>
-  </si>
-  <si>
-    <t>British comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British humour and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Movies and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jimi Hendrix</t>
-  </si>
-  <si>
-    <t>Rock music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Guitar music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing rock songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jon Stewart</t>
-  </si>
-  <si>
-    <t>Comedy Central and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Late-night TV and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the News and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Johnny Carson</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Stevie Wonder</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Law and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>chasing criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> interpreting evidence in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mother Teresa</t>
-  </si>
-  <si>
-    <t>Calcutta and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> India and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christianity and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Dan Quayle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>campaigning for the senate in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tony Soprano</t>
-  </si>
-  <si>
-    <t>the New Jersey Mob and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> New Jersey and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Mafia and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>JD Salinger</t>
-  </si>
-  <si>
-    <t>American literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>hiding from the public in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing modern fiction in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Matt "Daredevil" Murdock</t>
-  </si>
-  <si>
-    <t>Marvel Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>maintaining a secret identity in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pursuing criminals in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Michael Jackson</t>
-  </si>
-  <si>
-    <t>playing pop music in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> performing moon walks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jamie Oliver</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Howard Stern</t>
-  </si>
-  <si>
-    <t>Talk radio and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>shocking radio listeners in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hosting radio shows in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Dean Martin</t>
-  </si>
-  <si>
-    <t>Easy Listening and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Rat Pack and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing middle-of-the-road songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Kim Kardashian</t>
-  </si>
-  <si>
-    <t>Reality TV and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in reality TV shows in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> flaunting buttocks in Cthulhu-worshipping societies</t>
+    <t xml:space="preserve"> Krypton and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Science Fiction and the Dagon mythos</t>
   </si>
 </sst>
 </file>
@@ -789,7 +795,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>7.017471519938102E-6</v>
+        <v>6.971926933723982E-6</v>
       </c>
     </row>
     <row r="3">
@@ -803,7 +809,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>8.470385714357669E-6</v>
+        <v>8.406162144306703E-6</v>
       </c>
     </row>
     <row r="4">
@@ -817,7 +823,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.020096145586441E-5</v>
+        <v>1.0112760104766632E-5</v>
       </c>
     </row>
     <row r="5">
@@ -831,7 +837,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2257288749077716E-5</v>
+        <v>1.2138601491805891E-5</v>
       </c>
     </row>
     <row r="6">
@@ -845,7 +851,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>1.469478101524425E-5</v>
+        <v>1.4537663403317957E-5</v>
       </c>
     </row>
     <row r="7">
@@ -859,7 +865,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.757709949315312E-5</v>
+        <v>1.7371910019377772E-5</v>
       </c>
     </row>
     <row r="8">
@@ -870,10 +876,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D8" t="n">
-        <v>2.0977160184396766E-5</v>
+        <v>2.0712262413304845E-5</v>
       </c>
     </row>
     <row r="9">
@@ -884,10 +890,10 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D9" t="n">
-        <v>2.497822475773848E-5</v>
+        <v>2.4639648886750476E-5</v>
       </c>
     </row>
     <row r="10">
@@ -898,10 +904,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>2.9675075650580502E-5</v>
+        <v>2.9246136092987165E-5</v>
       </c>
     </row>
     <row r="11">
@@ -915,7 +921,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>3.517527419365113E-5</v>
+        <v>3.46361398816994E-5</v>
       </c>
     </row>
     <row r="12">
@@ -929,315 +935,315 @@
         <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>4.160049892369086E-5</v>
+        <v>4.092771323297849E-5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>4.908795932721859E-5</v>
+        <v>4.825390683763851E-5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D14" t="n">
-        <v>5.7791878069858376E-5</v>
+        <v>5.676419581900294E-5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D15" t="n">
-        <v>6.788503230894697E-5</v>
+        <v>6.662596377654371E-5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D16" t="n">
-        <v>7.956034196748987E-5</v>
+        <v>7.802603276866422E-5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>9.303248987731954E-5</v>
+        <v>9.117222505186369E-5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>1.0853955549992703E-4</v>
+        <v>1.0629493937539653E-4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>1.263446405345847E-4</v>
+        <v>1.2364872142239108E-4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D20" t="n">
-        <v>1.4673746116624037E-4</v>
+        <v>1.4351380462694846E-4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D21" t="n">
-        <v>1.7003587804090715E-4</v>
+        <v>1.6619759412949005E-4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D22" t="n">
-        <v>1.9658733134678944E-4</v>
+        <v>1.9203606311700883E-4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D23" t="n">
-        <v>2.2677014469946232E-4</v>
+        <v>2.2139502729944926E-4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C24" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D24" t="n">
-        <v>2.60994657963949E-4</v>
+        <v>2.5467125987688275E-4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>2.9970414579277567E-4</v>
+        <v>2.92293406144298E-4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D26" t="n">
-        <v>3.433754756229563E-4</v>
+        <v>3.3472265395979904E-4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D27" t="n">
-        <v>3.9251945627264816E-4</v>
+        <v>3.824531137760286E-4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D28" t="n">
-        <v>4.4768082623142637E-4</v>
+        <v>4.360118599168101E-4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D29" t="n">
-        <v>5.094378293764245E-4</v>
+        <v>4.959585833917476E-4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D30" t="n">
-        <v>5.784013252972359E-4</v>
+        <v>5.628848059011995E-4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D31" t="n">
-        <v>6.552133818083592E-4</v>
+        <v>6.374126049153057E-4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D32" t="n">
-        <v>7.40545298689348E-4</v>
+        <v>7.201928009306271E-4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D33" t="n">
-        <v>8.350950143424813E-4</v>
+        <v>8.11902560327927E-4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D34" t="n">
-        <v>9.395838509925402E-4</v>
+        <v>9.132423707729868E-4</v>
       </c>
     </row>
     <row r="35">
@@ -1245,13 +1251,13 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>11</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0010547525593680987</v>
+        <v>0.0010249323509077934</v>
       </c>
     </row>
     <row r="36">
@@ -1259,27 +1265,27 @@
         <v>51</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
         <v>11</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0011813566305575382</v>
+        <v>0.0011477078622304307</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
         <v>11</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0013201608509710548</v>
+        <v>0.0012823143986089025</v>
       </c>
     </row>
     <row r="38">
@@ -1287,13 +1293,13 @@
         <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0014719330860658124</v>
+        <v>0.0014295017378235797</v>
       </c>
     </row>
     <row r="39">
@@ -1301,27 +1307,27 @@
         <v>55</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0016374372896856663</v>
+        <v>0.0015900173498727115</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D40" t="n">
-        <v>0.001817425748460385</v>
+        <v>0.00176459906844984</v>
       </c>
     </row>
     <row r="41">
@@ -1329,181 +1335,181 @@
         <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0020126305846011917</v>
+        <v>0.0019539670449253144</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D42" t="n">
-        <v>0.002223754555467767</v>
+        <v>0.0021588150181977087</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D43" t="n">
-        <v>0.002451461204281951</v>
+        <v>0.002379800948768492</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0026963644330746</v>
+        <v>0.0026175370810999805</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0029590175861099847</v>
+        <v>0.0028725795145188443</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D46" t="n">
-        <v>0.003239902149308818</v>
+        <v>0.003145417379298042</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C47" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>0.003539416188222913</v>
+        <v>0.0034364617307992493</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C48" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>0.003857862663532177</v>
+        <v>0.0037460342902951305</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D49" t="n">
-        <v>0.004195437778405142</v>
+        <v>0.004074356175970038</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D50" t="n">
-        <v>0.004552219525981893</v>
+        <v>0.004421536781177238</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
-        <v>0.004928156617247825</v>
+        <v>0.004787562968970871</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
       </c>
       <c r="D52" t="n">
-        <v>0.005323057979264967</v>
+        <v>0.005172288761737642</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D53" t="n">
-        <v>0.005736583020676034</v>
+        <v>0.0055754257121434225</v>
       </c>
     </row>
     <row r="54">
@@ -1511,13 +1517,13 @@
         <v>77</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D54" t="n">
-        <v>0.006168232865249035</v>
+        <v>0.0059965341461159505</v>
       </c>
     </row>
     <row r="55">
@@ -1525,536 +1531,536 @@
         <v>77</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D55" t="n">
-        <v>0.0066173427545822006</v>
+        <v>0.006435015469944294</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>0.007083075817749196</v>
+        <v>0.006890105731457097</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>0.007564418398284034</v>
+        <v>0.0073608706194592255</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="n">
-        <v>0.008060177117463041</v>
+        <v>0.007846202075944275</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D59" t="n">
-        <v>0.008568977837176361</v>
+        <v>0.008344816682026523</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D60" t="n">
-        <v>0.00908926666586507</v>
+        <v>0.008855255961014386</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
         <v>88</v>
       </c>
       <c r="C61" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D61" t="n">
-        <v>0.009619313127185225</v>
+        <v>0.00937588872068884</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D62" t="n">
-        <v>0.010157215583416146</v>
+        <v>0.009904915531830372</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D63" t="n">
-        <v>0.010700908974553336</v>
+        <v>0.010440375411636227</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
         <v>92</v>
       </c>
       <c r="C64" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D64" t="n">
-        <v>0.011248174899929853</v>
+        <v>0.010980154749292481</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C65" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.01179665403260799</v>
+        <v>0.011521998477022233</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.012343860818350927</v>
+        <v>0.012063523454062086</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>0.012887200371360041</v>
+        <v>0.012602233993762813</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>0.013423987438968887</v>
+        <v>0.01313553942615353</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>0.013951467267896756</v>
+        <v>0.013660773550525751</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D70" t="n">
-        <v>0.014466838166334817</v>
+        <v>0.014175215795704799</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D71" t="n">
-        <v>0.014967275519946366</v>
+        <v>0.014676113870492169</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D72" t="n">
-        <v>0.015449956986596292</v>
+        <v>0.015160707654016836</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D73" t="n">
-        <v>0.015912088565157134</v>
+        <v>0.01562625404630022</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D74" t="n">
-        <v>0.01635093120877612</v>
+        <v>0.01607005247381435</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D75" t="n">
-        <v>0.01676382763322043</v>
+        <v>0.016489470724026956</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>0.017148228956951922</v>
+        <v>0.01688197076727571</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>0.017501720801841092</v>
+        <v>0.01724513421447693</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
-        <v>0.01782204848229782</v>
+        <v>0.017576687055348733</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D79" t="n">
-        <v>0.018107140916228656</v>
+        <v>0.017874523324380942</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D80" t="n">
-        <v>0.01835513290372419</v>
+        <v>0.018136727350762924</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D81" t="n">
-        <v>0.018564385438557388</v>
+        <v>0.018361594263842027</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>0.018733503743257836</v>
+        <v>0.01854764844730096</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>0.018861352750214153</v>
+        <v>0.018693659662711817</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
         <v>6</v>
       </c>
       <c r="D84" t="n">
-        <v>0.01894706978846155</v>
+        <v>0.018798656596063387</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C85" t="s">
         <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>0.018990074277792646</v>
+        <v>0.018861937618593047</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C86" t="s">
         <v>6</v>
       </c>
       <c r="D86" t="n">
-        <v>0.018990074277792465</v>
+        <v>0.018883078595161397</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>0.018947069788461564</v>
+        <v>0.01886193761859287</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B88" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C88" t="s">
         <v>11</v>
       </c>
       <c r="D88" t="n">
-        <v>0.018861352750213972</v>
+        <v>0.018798656596063397</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B89" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C89" t="s">
         <v>11</v>
       </c>
       <c r="D89" t="n">
-        <v>0.018733503743257822</v>
+        <v>0.018693659662711984</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B90" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C90" t="s">
         <v>11</v>
       </c>
       <c r="D90" t="n">
-        <v>0.01856438543855775</v>
+        <v>0.01854764844730096</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91" t="n">
-        <v>0.018355132903724022</v>
+        <v>0.018361594263841888</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B92" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
       </c>
       <c r="D92" t="n">
-        <v>0.018107140916228656</v>
+        <v>0.018136727350762896</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B93" t="s">
         <v>131</v>
@@ -2063,152 +2069,152 @@
         <v>11</v>
       </c>
       <c r="D93" t="n">
-        <v>0.01782204848229768</v>
+        <v>0.01787452332438111</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C94" t="s">
         <v>11</v>
       </c>
       <c r="D94" t="n">
-        <v>0.017501720801841064</v>
+        <v>0.017576687055348733</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B95" t="s">
         <v>134</v>
       </c>
       <c r="C95" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D95" t="n">
-        <v>0.017148228956952255</v>
+        <v>0.017245134214476876</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B96" t="s">
         <v>135</v>
       </c>
       <c r="C96" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D96" t="n">
-        <v>0.016763827633220346</v>
+        <v>0.016881970767275767</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C97" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D97" t="n">
-        <v>0.016350931208776093</v>
+        <v>0.016489470724026956</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B98" t="s">
         <v>138</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D98" t="n">
-        <v>0.015912088565157106</v>
+        <v>0.01607005247381435</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B99" t="s">
         <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D99" t="n">
-        <v>0.015449956986596125</v>
+        <v>0.015626254046300053</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B100" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C100" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D100" t="n">
-        <v>0.014967275519946643</v>
+        <v>0.015160707654017058</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B101" t="s">
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D101" t="n">
-        <v>0.014466838166334817</v>
+        <v>0.014676113870492169</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B102" t="s">
         <v>143</v>
       </c>
       <c r="C102" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D102" t="n">
-        <v>0.013951467267896644</v>
+        <v>0.014175215795704688</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B103" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C103" t="s">
         <v>11</v>
       </c>
       <c r="D103" t="n">
-        <v>0.013423987438968887</v>
+        <v>0.01366077355052564</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B104" t="s">
         <v>146</v>
@@ -2217,12 +2223,12 @@
         <v>11</v>
       </c>
       <c r="D104" t="n">
-        <v>0.012887200371359875</v>
+        <v>0.013135539426153753</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B105" t="s">
         <v>147</v>
@@ -2231,68 +2237,68 @@
         <v>11</v>
       </c>
       <c r="D105" t="n">
-        <v>0.012343860818351204</v>
+        <v>0.012602233993762813</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B106" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C106" t="s">
         <v>11</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01179665403260799</v>
+        <v>0.01206352345406203</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B107" t="s">
         <v>150</v>
       </c>
       <c r="C107" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D107" t="n">
-        <v>0.011248174899929742</v>
+        <v>0.011521998477022288</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B108" t="s">
         <v>151</v>
       </c>
       <c r="C108" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D108" t="n">
-        <v>0.010700908974553336</v>
+        <v>0.010980154749292481</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B109" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C109" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D109" t="n">
-        <v>0.010157215583416146</v>
+        <v>0.010440375411636171</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B110" t="s">
         <v>154</v>
@@ -2301,12 +2307,12 @@
         <v>6</v>
       </c>
       <c r="D110" t="n">
-        <v>0.00961931312718517</v>
+        <v>0.009904915531830205</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B111" t="s">
         <v>155</v>
@@ -2315,26 +2321,26 @@
         <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>0.009089266665865237</v>
+        <v>0.009375888720689063</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B112" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C112" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D112" t="n">
-        <v>0.008568977837176361</v>
+        <v>0.008855255961014386</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B113" t="s">
         <v>158</v>
@@ -2343,12 +2349,12 @@
         <v>11</v>
       </c>
       <c r="D113" t="n">
-        <v>0.008060177117463041</v>
+        <v>0.008344816682026468</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B114" t="s">
         <v>159</v>
@@ -2357,7 +2363,7 @@
         <v>11</v>
       </c>
       <c r="D114" t="n">
-        <v>0.0075644183982837565</v>
+        <v>0.007846202075944164</v>
       </c>
     </row>
     <row r="115">
@@ -2368,10 +2374,10 @@
         <v>161</v>
       </c>
       <c r="C115" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D115" t="n">
-        <v>0.007083075817749307</v>
+        <v>0.007360870619459392</v>
       </c>
     </row>
     <row r="116">
@@ -2382,10 +2388,10 @@
         <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D116" t="n">
-        <v>0.006617342754582367</v>
+        <v>0.006890105731457097</v>
       </c>
     </row>
     <row r="117">
@@ -2396,10 +2402,10 @@
         <v>163</v>
       </c>
       <c r="C117" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D117" t="n">
-        <v>0.006168232865249035</v>
+        <v>0.0064350154699442386</v>
       </c>
     </row>
     <row r="118">
@@ -2410,10 +2416,10 @@
         <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D118" t="n">
-        <v>0.005736583020675756</v>
+        <v>0.005996534146116006</v>
       </c>
     </row>
     <row r="119">
@@ -2424,10 +2430,10 @@
         <v>166</v>
       </c>
       <c r="C119" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D119" t="n">
-        <v>0.005323057979265022</v>
+        <v>0.0055754257121434225</v>
       </c>
     </row>
     <row r="120">
@@ -2438,10 +2444,10 @@
         <v>167</v>
       </c>
       <c r="C120" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>0.004928156617248103</v>
+        <v>0.005172288761737587</v>
       </c>
     </row>
     <row r="121">
@@ -2455,7 +2461,7 @@
         <v>6</v>
       </c>
       <c r="D121" t="n">
-        <v>0.004552219525981727</v>
+        <v>0.004787562968970982</v>
       </c>
     </row>
     <row r="122">
@@ -2469,7 +2475,7 @@
         <v>6</v>
       </c>
       <c r="D122" t="n">
-        <v>0.004195437778405253</v>
+        <v>0.004421536781177182</v>
       </c>
     </row>
     <row r="123">
@@ -2483,7 +2489,7 @@
         <v>6</v>
       </c>
       <c r="D123" t="n">
-        <v>0.003857862663532108</v>
+        <v>0.004074356175970038</v>
       </c>
     </row>
     <row r="124">
@@ -2494,10 +2500,10 @@
         <v>173</v>
       </c>
       <c r="C124" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D124" t="n">
-        <v>0.003539416188222941</v>
+        <v>0.003746034290295089</v>
       </c>
     </row>
     <row r="125">
@@ -2508,10 +2514,10 @@
         <v>174</v>
       </c>
       <c r="C125" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D125" t="n">
-        <v>0.003239902149308787</v>
+        <v>0.003436461730799263</v>
       </c>
     </row>
     <row r="126">
@@ -2522,10 +2528,10 @@
         <v>175</v>
       </c>
       <c r="C126" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D126" t="n">
-        <v>0.0029590175861099882</v>
+        <v>0.0031454173792980697</v>
       </c>
     </row>
     <row r="127">
@@ -2536,10 +2542,10 @@
         <v>177</v>
       </c>
       <c r="C127" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0026963644330746696</v>
+        <v>0.0028725795145188443</v>
       </c>
     </row>
     <row r="128">
@@ -2550,10 +2556,10 @@
         <v>178</v>
       </c>
       <c r="C128" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D128" t="n">
-        <v>0.002451461204281951</v>
+        <v>0.00261753708109997</v>
       </c>
     </row>
     <row r="129">
@@ -2564,10 +2570,10 @@
         <v>179</v>
       </c>
       <c r="C129" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0022237545554677357</v>
+        <v>0.0023798009487685026</v>
       </c>
     </row>
     <row r="130">
@@ -2581,7 +2587,7 @@
         <v>6</v>
       </c>
       <c r="D130" t="n">
-        <v>0.002012630584601164</v>
+        <v>0.0021588150181977087</v>
       </c>
     </row>
     <row r="131">
@@ -2595,7 +2601,7 @@
         <v>6</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0018174257484604387</v>
+        <v>0.0019539670449252797</v>
       </c>
     </row>
     <row r="132">
@@ -2609,7 +2615,7 @@
         <v>6</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0016374372896856716</v>
+        <v>0.0017645990684498746</v>
       </c>
     </row>
     <row r="133">
@@ -2623,7 +2629,7 @@
         <v>6</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0014719330860658124</v>
+        <v>0.0015900173498727115</v>
       </c>
     </row>
     <row r="134">
@@ -2637,7 +2643,7 @@
         <v>6</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0013201608509710513</v>
+        <v>0.0014295017378235797</v>
       </c>
     </row>
     <row r="135">
@@ -2651,7 +2657,7 @@
         <v>6</v>
       </c>
       <c r="D135" t="n">
-        <v>0.0011813566305575226</v>
+        <v>0.0012823143986088973</v>
       </c>
     </row>
     <row r="136">
@@ -2662,66 +2668,66 @@
         <v>189</v>
       </c>
       <c r="C136" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D136" t="n">
-        <v>0.00105475255936809</v>
+        <v>0.001147707862230436</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
+        <v>188</v>
+      </c>
+      <c r="B137" t="s">
         <v>190</v>
       </c>
-      <c r="B137" t="s">
-        <v>191</v>
-      </c>
       <c r="C137" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D137" t="n">
-        <v>9.39583850992568E-4</v>
+        <v>0.0010249323509077934</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>160</v>
+        <v>188</v>
       </c>
       <c r="B138" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C138" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D138" t="n">
-        <v>8.350950143424813E-4</v>
+        <v>9.132423707729868E-4</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="B139" t="s">
         <v>193</v>
       </c>
       <c r="C139" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D139" t="n">
-        <v>7.405452986893385E-4</v>
+        <v>8.119025603279106E-4</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>160</v>
+        <v>192</v>
       </c>
       <c r="B140" t="s">
         <v>194</v>
       </c>
       <c r="C140" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D140" t="n">
-        <v>6.552133818083575E-4</v>
+        <v>7.201928009306436E-4</v>
       </c>
     </row>
     <row r="141">
@@ -2732,10 +2738,10 @@
         <v>196</v>
       </c>
       <c r="C141" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D141" t="n">
-        <v>5.784013252972415E-4</v>
+        <v>6.374126049153057E-4</v>
       </c>
     </row>
     <row r="142">
@@ -2746,10 +2752,10 @@
         <v>197</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D142" t="n">
-        <v>5.094378293764197E-4</v>
+        <v>5.628848059011935E-4</v>
       </c>
     </row>
     <row r="143">
@@ -2760,10 +2766,10 @@
         <v>198</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D143" t="n">
-        <v>4.476808262314368E-4</v>
+        <v>4.959585833917532E-4</v>
       </c>
     </row>
     <row r="144">
@@ -2777,7 +2783,7 @@
         <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>3.9251945627264816E-4</v>
+        <v>4.3601185991681054E-4</v>
       </c>
     </row>
     <row r="145">
@@ -2791,54 +2797,54 @@
         <v>6</v>
       </c>
       <c r="D145" t="n">
-        <v>3.433754756229563E-4</v>
+        <v>3.824531137760286E-4</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
+        <v>199</v>
+      </c>
+      <c r="B146" t="s">
         <v>202</v>
       </c>
-      <c r="B146" t="s">
-        <v>203</v>
-      </c>
       <c r="C146" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D146" t="n">
-        <v>2.997041457927683E-4</v>
+        <v>3.3472265395979904E-4</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B147" t="s">
         <v>204</v>
       </c>
       <c r="C147" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D147" t="n">
-        <v>2.6099465796395336E-4</v>
+        <v>2.92293406144298E-4</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B148" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C148" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D148" t="n">
-        <v>2.2677014469946535E-4</v>
+        <v>2.5467125987688275E-4</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B149" t="s">
         <v>207</v>
@@ -2847,12 +2853,12 @@
         <v>6</v>
       </c>
       <c r="D149" t="n">
-        <v>1.9658733134678944E-4</v>
+        <v>2.2139502729944926E-4</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B150" t="s">
         <v>208</v>
@@ -2861,152 +2867,152 @@
         <v>6</v>
       </c>
       <c r="D150" t="n">
-        <v>1.7003587804090455E-4</v>
+        <v>1.9203606311700883E-4</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="B151" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C151" t="s">
         <v>6</v>
       </c>
       <c r="D151" t="n">
-        <v>1.467374611662407E-4</v>
+        <v>1.6619759412949005E-4</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B152" t="s">
         <v>211</v>
       </c>
       <c r="C152" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D152" t="n">
-        <v>1.2634464053458568E-4</v>
+        <v>1.4351380462694846E-4</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B153" t="s">
         <v>212</v>
       </c>
       <c r="C153" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D153" t="n">
-        <v>1.0853955549992519E-4</v>
+        <v>1.2364872142239065E-4</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B154" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C154" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D154" t="n">
-        <v>9.303248987732268E-5</v>
+        <v>1.0629493937539696E-4</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B155" t="s">
         <v>215</v>
       </c>
       <c r="C155" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D155" t="n">
-        <v>7.956034196748856E-5</v>
+        <v>9.117222505186369E-5</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C156" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D156" t="n">
-        <v>6.788503230894827E-5</v>
+        <v>7.802603276866422E-5</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B157" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C157" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D157" t="n">
-        <v>5.779187806985691E-5</v>
+        <v>6.66259637765423E-5</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B158" t="s">
         <v>219</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D158" t="n">
-        <v>4.9087959327219564E-5</v>
+        <v>5.676419581900435E-5</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B159" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C159" t="s">
         <v>6</v>
       </c>
       <c r="D159" t="n">
-        <v>4.160049892369135E-5</v>
+        <v>4.825390683763851E-5</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="B160" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C160" t="s">
         <v>6</v>
       </c>
       <c r="D160" t="n">
-        <v>3.517527419365113E-5</v>
+        <v>4.092771323297849E-5</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B161" t="s">
         <v>223</v>
@@ -3015,82 +3021,82 @@
         <v>6</v>
       </c>
       <c r="D161" t="n">
-        <v>2.967507565058007E-5</v>
+        <v>3.463613988169908E-5</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B162" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C162" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D162" t="n">
-        <v>2.497822475773867E-5</v>
+        <v>2.924613609298749E-5</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B163" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C163" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D163" t="n">
-        <v>2.097716018439636E-5</v>
+        <v>2.4639648886750476E-5</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B164" t="s">
         <v>227</v>
       </c>
       <c r="C164" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D164" t="n">
-        <v>1.757709949315377E-5</v>
+        <v>2.0712262413304574E-5</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B165" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C165" t="s">
         <v>6</v>
       </c>
       <c r="D165" t="n">
-        <v>1.469478101524425E-5</v>
+        <v>1.7371910019377786E-5</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B166" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C166" t="s">
         <v>6</v>
       </c>
       <c r="D166" t="n">
-        <v>1.2257288749077526E-5</v>
+        <v>1.4537663403318214E-5</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B167" t="s">
         <v>231</v>
@@ -3099,35 +3105,49 @@
         <v>6</v>
       </c>
       <c r="D167" t="n">
-        <v>1.0200961455864424E-5</v>
+        <v>1.2138601491805891E-5</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B168" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C168" t="s">
         <v>6</v>
       </c>
       <c r="D168" t="n">
-        <v>8.470385714357743E-6</v>
+        <v>1.0112760104766496E-5</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B169" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C169" t="s">
         <v>6</v>
       </c>
       <c r="D169" t="n">
-        <v>7.017471519938204E-6</v>
+        <v>8.40616214430677E-6</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="s">
+        <v>232</v>
+      </c>
+      <c r="B170" t="s">
+        <v>235</v>
+      </c>
+      <c r="C170" t="s">
+        <v>6</v>
+      </c>
+      <c r="D170" t="n">
+        <v>6.97192693372405E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added project preference assignment to application
</commit_message>
<xml_diff>
--- a/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
+++ b/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="237">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,33 +26,243 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Lara Croft</t>
-  </si>
-  <si>
-    <t>Tomb Raider and the Dagon mythos</t>
+    <t>Will Smith</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Lt. George Colthurst St Barleigh</t>
+  </si>
+  <si>
+    <t>the English class system and the Dagon mythos</t>
   </si>
   <si>
     <t>DS</t>
   </si>
   <si>
-    <t>looking for hidden treasures in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>unearthing ancient tombs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Fred Astaire</t>
-  </si>
-  <si>
-    <t>Dancing and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>CS</t>
+    <t>providing comic relief in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bruce Wayne</t>
+  </si>
+  <si>
+    <t>DC Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Big business and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gotham City and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Princess Diana</t>
+  </si>
+  <si>
+    <t>Politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British royalty and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British history and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Serena Williams</t>
+  </si>
+  <si>
+    <t>Tennis and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>delivering forehand slams in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> winning tennis tournaments in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jonathan Swift</t>
+  </si>
+  <si>
+    <t>Satire and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Irish Famine and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing political satires in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Billy Crystal</t>
+  </si>
+  <si>
+    <t>American comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American culture and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Nicolas Cage</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Action movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Deadpool</t>
+  </si>
+  <si>
+    <t>Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The X-Men and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Michael J. Fox</t>
+  </si>
+  <si>
+    <t>Back To The Future and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Family Ties and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spin City and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Jenna Maroney</t>
+  </si>
+  <si>
+    <t>30 Rock and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Television Production and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Deepak Chopra</t>
+  </si>
+  <si>
+    <t>Eastern philosophy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Self-Help and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting Eastern philosophy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing mystery stories in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dolly Parton</t>
+  </si>
+  <si>
+    <t>Country music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing country music in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Tina Turner</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Frank Zappa</t>
+  </si>
+  <si>
+    <t>Experimental music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing experimental songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing experimental songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ray Kroc</t>
+  </si>
+  <si>
+    <t>McDonalds and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Hamburger industry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a multinational corporation in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Barry White</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Love songs and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing romantic songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Paris Hilton</t>
+  </si>
+  <si>
+    <t>Reality TV and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>monetizing celebrity status in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making unauthorized sex tapes in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joan Crawford</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu mythos</t>
   </si>
   <si>
     <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
   </si>
   <si>
+    <t>Hugh Grant</t>
+  </si>
+  <si>
     <t>starring in romantic comedies in Cthulhu-worshipping societies</t>
   </si>
   <si>
@@ -68,73 +278,43 @@
     <t xml:space="preserve"> killing murderers in Dagon-worshipping societies</t>
   </si>
   <si>
-    <t>Dave Lee Roth</t>
-  </si>
-  <si>
-    <t>Rock music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing rock songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Enrico Caruso</t>
-  </si>
-  <si>
-    <t>Opera and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t>singing opera arias in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Janis Joplin</t>
-  </si>
-  <si>
-    <t>Psychadelic music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tony Stark</t>
-  </si>
-  <si>
-    <t>Marvel Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Technology and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a multinational corporation in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pablo Escobar</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> International Crime and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a criminal enterprise in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> running a crime family in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Barney Gumble</t>
-  </si>
-  <si>
-    <t>The Simpsons and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>drinking one's life away in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mike  Pence</t>
+    <t>Rembrandt</t>
+  </si>
+  <si>
+    <t>Painting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>painting colorful pictures in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> painting self-portraits in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Cher</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joaquin Phoenix</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serious Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>starring in action movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in indy movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sean Hannity</t>
   </si>
   <si>
     <t>the Right and the Cthulu-Dagon mythos</t>
@@ -146,580 +326,403 @@
     <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t>Coco Chanel</t>
-  </si>
-  <si>
-    <t>Fashion and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Rag Trade and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Fashion industry and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Edith Piaf</t>
-  </si>
-  <si>
-    <t>Cabaret singing and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing melancholy songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Kylie Minogue</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pythagoras</t>
-  </si>
-  <si>
-    <t>Mathematics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ancient Greece and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>studying mathematics in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ilya Kuryakin</t>
-  </si>
-  <si>
-    <t>The Man from U.N.C.L.E and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Hillary Clinton</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Left and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Democrats and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Willie Nelson</t>
-  </si>
-  <si>
-    <t>Country music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing country music in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Waylon Smithers</t>
-  </si>
-  <si>
-    <t>Nuclear Power and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Simpsons and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fawning on the boss in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Thomas Edison</t>
-  </si>
-  <si>
-    <t>Physics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>pioneering new technologies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>LeBron James</t>
-  </si>
-  <si>
-    <t>Basketball and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>playing basketball in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making dunk shots in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Princess Leia Organa</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>leading the rebel alliance in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> smuggling military plans in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pocahontas</t>
-  </si>
-  <si>
-    <t>American history and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the New world and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>bridging cultures  in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>G. Gordon Liddy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ranting about liberals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bugging political rivals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pulling dirty political tricks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Professor Hans Zarkov</t>
-  </si>
-  <si>
-    <t>Flash Gordon and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>building rocket ships in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Doc Emmett Brown</t>
+    <t>Samson</t>
+  </si>
+  <si>
+    <t>the Bible and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Old Testament and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judaism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Marty McFly</t>
   </si>
   <si>
     <t>Back To The Future and the Dagon mythos</t>
   </si>
   <si>
-    <t>pioneering new technologies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> developing new technologies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>William Randolph Hearst</t>
-  </si>
-  <si>
-    <t>the Newspaper industry and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a media empire in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> publishing newspapers in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Larry Flynt</t>
-  </si>
-  <si>
-    <t>Hustler Magazine and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soft pornography and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>publishing soft pornography in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Samwise Gamgee</t>
-  </si>
-  <si>
-    <t>The Lord of the Rings and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Hobbit and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>tending the garden in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Babe Ruth</t>
-  </si>
-  <si>
-    <t>Baseball and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American sports and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>hitting home runs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Polonius</t>
-  </si>
-  <si>
-    <t>Denmark and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Elsinore and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hamlet: Prince of Denmark and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Selma Bouvier</t>
-  </si>
-  <si>
-    <t>smoking Laramie Hi-Tars in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> watching MacGyver reruns in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> clipping coupons in Dagon-worshipping societies</t>
+    <t>playing rock music in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> playing rock guitar in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Monsieur Hulot</t>
+  </si>
+  <si>
+    <t>French comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> French humour and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>causing mayhem in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ben Affleck</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making bad movie choices in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Pablo Picasso</t>
+  </si>
+  <si>
+    <t>Modern art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cubism and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>painting abstract pictures in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Gwyneth Paltrow</t>
+  </si>
+  <si>
+    <t>running a new-age website in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> raising new-age children in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ebenezer Scrooge</t>
+  </si>
+  <si>
+    <t>A Christmas Carol and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Benny Hill</t>
+  </si>
+  <si>
+    <t>British comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British humour and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>chasing old women in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Monica Lewinsky</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Clinton Era and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>conducting illicit affairs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stewie Griffin</t>
+  </si>
+  <si>
+    <t>Family Guy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>plotting against family members in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pioneering new technologies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jeff Koons</t>
+  </si>
+  <si>
+    <t>American art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making modern art in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dr. John Watson</t>
+  </si>
+  <si>
+    <t>Sherlock Holmes and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Detective fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>chasing criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Carrie Bradshaw</t>
+  </si>
+  <si>
+    <t>Sex and the City and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Manhattan and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing about sex in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Yosemite Sam</t>
+  </si>
+  <si>
+    <t>Looney Tunes and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Warner Bros animation and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>losing control in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Aristotle</t>
+  </si>
+  <si>
+    <t>Ancient philosophy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Greek philosophy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Ancient world and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Judge Joe Dredd</t>
+  </si>
+  <si>
+    <t>Mega-City One and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>tracking down criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> preventing crime in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Leon Trotsky</t>
+  </si>
+  <si>
+    <t>the Russian revolution and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>spreading revolution in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> promoting communism in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
   </si>
   <si>
     <t>Jim Carrey</t>
   </si>
   <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>gurning for the camera in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Savonarola</t>
-  </si>
-  <si>
-    <t>Florence and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Renaissance and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Kenny G</t>
-  </si>
-  <si>
-    <t>Easy Listening and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Light Jazz and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Saxophone music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Deep Throat</t>
-  </si>
-  <si>
-    <t>Watergate and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>talking in riddles in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> offering advice in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Keyser Söze</t>
-  </si>
-  <si>
-    <t>The Usual Suspects and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a criminal enterprise in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> eluding the FBI in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Reince Priebus</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
+    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>gurning for the camera in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pulling faces in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Chandler Bing</t>
+  </si>
+  <si>
+    <t>Friends and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>making sarcastic remarks in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Trinity</t>
+  </si>
+  <si>
+    <t>The Matrix and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>hacking into corporate mainframes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dante Alighieri</t>
+  </si>
+  <si>
+    <t>Italian literature and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Italian poetry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing poetry in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Rocket Raccoon</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Guardians of the Galaxy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>guarding the galaxy in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jack Sparrow</t>
+  </si>
+  <si>
+    <t>Pirates of the Carribean and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>collecting pirate booty in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> commanding a pirate ship in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>H.A.L. 9000</t>
+  </si>
+  <si>
+    <t>2001: A Space Odyssey and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Homicidal computers and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>murdering astronauts in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joan Rivers</t>
+  </si>
+  <si>
+    <t>Comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>insulting celebrities in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> doing stand-up in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>James Cook</t>
+  </si>
+  <si>
+    <t>British history and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>opening new markets in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exploring foreign countries in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Charles Lindbergh</t>
+  </si>
+  <si>
+    <t>Aviation and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American history and the Cthulu mythos</t>
   </si>
   <si>
     <t xml:space="preserve"> American politics and the Cthulu mythos</t>
   </si>
   <si>
-    <t>Jimi Hendrix</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Guitar music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> playing rock guitar in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Uriah Heap</t>
-  </si>
-  <si>
-    <t>David Copperfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Bette Midler</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing torch songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> over-acting in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Daniel Craig</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> James Bond and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in action movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in indy movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Philip Marlowe</t>
-  </si>
-  <si>
-    <t>Detective fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>solving mysteries in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Judge Joe Dredd</t>
-  </si>
-  <si>
-    <t>Mega-City One and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>tracking down criminals in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> preventing crime in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Stephen Hawking</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Modern science and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Cosmos and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting science in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Indiana Jones</t>
-  </si>
-  <si>
-    <t>Raiders of the Lost Ark and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Archeology and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> punching out Nazis in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Captain Ahab</t>
-  </si>
-  <si>
-    <t>Moby Dick and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Whaling and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>chasing a great white whale in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Monsieur Hulot</t>
-  </si>
-  <si>
-    <t>French comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> French humour and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>causing mayhem in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Helen Keller</t>
-  </si>
-  <si>
-    <t>American education and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>reading braille in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> avoiding eye contact in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Rico Tubbs</t>
-  </si>
-  <si>
-    <t>Miami Vice and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> arresting drug dealers in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Lynch</t>
-  </si>
-  <si>
-    <t>Movies and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Twin Peaks and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>directing weird movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Dorian Gray</t>
-  </si>
-  <si>
-    <t>The Picture of Dorian Gray and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>gadding about town in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> practicing good skin care in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>John Calvin</t>
-  </si>
-  <si>
-    <t>Religious Iconology and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Hans Gruber</t>
-  </si>
-  <si>
-    <t>Die Hard and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Nakatomi building and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>organizing armed robberies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Buffy Summers</t>
-  </si>
-  <si>
-    <t>Horror and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>hunting demons in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> hunting monsters in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Stanley Kowalski</t>
-  </si>
-  <si>
-    <t>A Street Car Named Desire and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>moaning about women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Lee Marvin</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> War movies and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Shylock</t>
-  </si>
-  <si>
-    <t>Shakespeare and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>amassing wealth in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> seeking revenge in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Roseanne Barr</t>
-  </si>
-  <si>
-    <t>Televison and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making vulgar jokes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Santa Claus</t>
-  </si>
-  <si>
-    <t>the North Pole and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christmas and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>delivering presents in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>General Zod</t>
-  </si>
-  <si>
-    <t>DC Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Krypton and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Science Fiction and the Dagon mythos</t>
+    <t>Federico Fellini</t>
+  </si>
+  <si>
+    <t>Italian Neo-realism and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making new wave movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making Italian movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bridget Jones</t>
+  </si>
+  <si>
+    <t>British culture and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>keeping a diary in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> moaning about men in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Kim Jung-un</t>
+  </si>
+  <si>
+    <t>Politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terrorism and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Asian politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Al Capone</t>
+  </si>
+  <si>
+    <t>Prohibition and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Mafia and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chicago and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Bradley Manning</t>
+  </si>
+  <si>
+    <t>Espionage and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wikileaks and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Michael Schumacher</t>
+  </si>
+  <si>
+    <t>Formula One and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Car Racing and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>driving fast cars in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Cicero</t>
+  </si>
+  <si>
+    <t>Oratory and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rhetoric and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ancient Rome and the Cthulu-Dagon mythos</t>
   </si>
 </sst>
 </file>
@@ -795,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>6.971926933723982E-6</v>
+        <v>6.926967971821188E-6</v>
       </c>
     </row>
     <row r="3">
@@ -809,7 +812,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>8.406162144306703E-6</v>
+        <v>8.342881412648925E-6</v>
       </c>
     </row>
     <row r="4">
@@ -823,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0112760104766632E-5</v>
+        <v>1.0025992586088537E-5</v>
       </c>
     </row>
     <row r="5">
@@ -837,7 +840,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2138601491805891E-5</v>
+        <v>1.2022010572145957E-5</v>
       </c>
     </row>
     <row r="6">
@@ -851,91 +854,91 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>1.4537663403317957E-5</v>
+        <v>1.4383522258392336E-5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.7371910019377772E-5</v>
+        <v>1.717085068725874E-5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>2.0712262413304845E-5</v>
+        <v>2.0452989317283098E-5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>2.4639648886750476E-5</v>
+        <v>2.430861353215688E-5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="n">
-        <v>2.9246136092987165E-5</v>
+        <v>2.8827169684496502E-5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
-        <v>3.46361398816994E-5</v>
+        <v>3.411004070620922E-5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D12" t="n">
-        <v>4.092771323297849E-5</v>
+        <v>4.027178584150283E-5</v>
       </c>
     </row>
     <row r="13">
@@ -949,7 +952,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>4.825390683763851E-5</v>
+        <v>4.744145035201822E-5</v>
       </c>
     </row>
     <row r="14">
@@ -963,26 +966,26 @@
         <v>23</v>
       </c>
       <c r="D14" t="n">
-        <v>5.676419581900294E-5</v>
+        <v>5.576393910025932E-5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
       <c r="C15" t="s">
         <v>23</v>
       </c>
       <c r="D15" t="n">
-        <v>6.662596377654371E-5</v>
+        <v>6.540144573573324E-5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
@@ -991,40 +994,40 @@
         <v>23</v>
       </c>
       <c r="D16" t="n">
-        <v>7.802603276866422E-5</v>
+        <v>7.653492679195325E-5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
         <v>28</v>
       </c>
-      <c r="B17" t="s">
-        <v>29</v>
-      </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D17" t="n">
-        <v>9.117222505186369E-5</v>
+        <v>8.936560736178727E-5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D18" t="n">
-        <v>1.0629493937539653E-4</v>
+        <v>1.0411650217097301E-4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
         <v>31</v>
@@ -1033,40 +1036,40 @@
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>1.2364872142239108E-4</v>
+        <v>1.2103393284026791E-4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" t="s">
-        <v>33</v>
-      </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>1.4351380462694846E-4</v>
+        <v>1.4038901894977706E-4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>1.6619759412949005E-4</v>
+        <v>1.624791172377655E-4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
@@ -1075,488 +1078,488 @@
         <v>23</v>
       </c>
       <c r="D22" t="n">
-        <v>1.9203606311700883E-4</v>
+        <v>1.876291799340331E-4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
         <v>36</v>
       </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D23" t="n">
-        <v>2.2139502729944926E-4</v>
+        <v>2.1619299990756563E-4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D24" t="n">
-        <v>2.5467125987688275E-4</v>
+        <v>2.485543070728921E-4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
         <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D25" t="n">
-        <v>2.92293406144298E-4</v>
+        <v>2.8512767743184655E-4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" t="s">
         <v>40</v>
       </c>
-      <c r="B26" t="s">
-        <v>41</v>
-      </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
-        <v>3.3472265395979904E-4</v>
+        <v>3.2635921331940166E-4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D27" t="n">
-        <v>3.824531137760286E-4</v>
+        <v>3.7272695097251935E-4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>4.360118599168101E-4</v>
+        <v>4.24740949557632E-4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
         <v>44</v>
       </c>
-      <c r="B29" t="s">
-        <v>45</v>
-      </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>4.959585833917476E-4</v>
+        <v>4.82943014384262E-4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>5.628848059011995E-4</v>
+        <v>5.479060063160461E-4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
-        <v>6.374126049153057E-4</v>
+        <v>6.202326894772089E-4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
         <v>48</v>
       </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="n">
-        <v>7.201928009306271E-4</v>
+        <v>7.005540703561072E-4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="n">
-        <v>8.11902560327927E-4</v>
+        <v>7.895271834311036E-4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
         <v>51</v>
       </c>
-      <c r="B34" t="s">
-        <v>52</v>
-      </c>
       <c r="C34" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D34" t="n">
-        <v>9.132423707729868E-4</v>
+        <v>8.878322815843278E-4</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0010249323509077934</v>
+        <v>9.961693939075107E-4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0011477078622304307</v>
+        <v>0.0011152542191052942</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0012823143986089025</v>
+        <v>0.0012458133296105577</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0014295017378235797</v>
+        <v>0.001388578669758526</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
         <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0015900173498727115</v>
+        <v>0.0015442813409155993</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" t="s">
         <v>59</v>
       </c>
-      <c r="B40" t="s">
-        <v>60</v>
-      </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="n">
-        <v>0.00176459906844984</v>
+        <v>0.0017136446772780915</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0019539670449253144</v>
+        <v>0.0018973766280731448</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42" t="s">
         <v>62</v>
       </c>
-      <c r="B42" t="s">
-        <v>63</v>
-      </c>
       <c r="C42" t="s">
         <v>23</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0021588150181977087</v>
+        <v>0.0020961614749889883</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
         <v>23</v>
       </c>
       <c r="D43" t="n">
-        <v>0.002379800948768492</v>
+        <v>0.0023106509276930483</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0026175370810999805</v>
+        <v>0.0025414546550541935</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" t="s">
         <v>66</v>
       </c>
-      <c r="B45" t="s">
-        <v>67</v>
-      </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0028725795145188443</v>
+        <v>0.002789130324967217</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D46" t="n">
-        <v>0.003145417379298042</v>
+        <v>0.0030541732411913276</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" t="s">
         <v>69</v>
       </c>
-      <c r="B47" t="s">
-        <v>70</v>
-      </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0034364617307992493</v>
+        <v>0.003337005681083534</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0037460342902951305</v>
+        <v>0.003637966053188099</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D49" t="n">
-        <v>0.004074356175970038</v>
+        <v>0.003957298007991987</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" t="s">
         <v>73</v>
       </c>
-      <c r="B50" t="s">
-        <v>74</v>
-      </c>
       <c r="C50" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D50" t="n">
-        <v>0.004421536781177238</v>
+        <v>0.004295139648408386</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C51" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D51" t="n">
-        <v>0.004787562968970871</v>
+        <v>0.004651512998309848</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>0.005172288761737642</v>
+        <v>0.005026313897343981</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
         <v>77</v>
       </c>
-      <c r="B53" t="s">
-        <v>78</v>
-      </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>0.0055754257121434225</v>
+        <v>0.005419302497937595</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0059965341461159505</v>
+        <v>0.005830094545484554</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B55" t="s">
         <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D55" t="n">
-        <v>0.006435015469944294</v>
+        <v>0.006258153624912388</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" t="s">
         <v>81</v>
       </c>
-      <c r="B56" t="s">
-        <v>82</v>
-      </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>0.006890105731457097</v>
+        <v>0.006702784555806973</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
         <v>83</v>
@@ -1565,68 +1568,68 @@
         <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>0.0073608706194592255</v>
+        <v>0.007163128113875039</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D58" t="n">
-        <v>0.007846202075944275</v>
+        <v>0.007638157248494426</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" t="s">
         <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D59" t="n">
-        <v>0.008344816682026523</v>
+        <v>0.00812667495442776</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
         <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D60" t="n">
-        <v>0.008855255961014386</v>
+        <v>0.008627313940323456</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
         <v>23</v>
       </c>
       <c r="D61" t="n">
-        <v>0.00937588872068884</v>
+        <v>0.009138538217574543</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
         <v>90</v>
@@ -1635,12 +1638,12 @@
         <v>23</v>
       </c>
       <c r="D62" t="n">
-        <v>0.009904915531830372</v>
+        <v>0.009658646710481888</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
         <v>91</v>
@@ -1649,26 +1652,26 @@
         <v>23</v>
       </c>
       <c r="D63" t="n">
-        <v>0.010440375411636227</v>
+        <v>0.01018577896280709</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C64" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>0.010980154749292481</v>
+        <v>0.010717922986950623</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
         <v>94</v>
@@ -1677,12 +1680,12 @@
         <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.011521998477022233</v>
+        <v>0.01125292527060301</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
         <v>95</v>
@@ -1691,7 +1694,7 @@
         <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.012063523454062086</v>
+        <v>0.011788502922287947</v>
       </c>
     </row>
     <row r="67">
@@ -1702,10 +1705,10 @@
         <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D67" t="n">
-        <v>0.012602233993762813</v>
+        <v>0.012322257902281752</v>
       </c>
     </row>
     <row r="68">
@@ -1716,10 +1719,10 @@
         <v>98</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D68" t="n">
-        <v>0.01313553942615353</v>
+        <v>0.012851693249620766</v>
       </c>
     </row>
     <row r="69">
@@ -1730,10 +1733,10 @@
         <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D69" t="n">
-        <v>0.013660773550525751</v>
+        <v>0.013374231179969054</v>
       </c>
     </row>
     <row r="70">
@@ -1747,7 +1750,7 @@
         <v>23</v>
       </c>
       <c r="D70" t="n">
-        <v>0.014175215795704799</v>
+        <v>0.013887232893715129</v>
       </c>
     </row>
     <row r="71">
@@ -1761,7 +1764,7 @@
         <v>23</v>
       </c>
       <c r="D71" t="n">
-        <v>0.014676113870492169</v>
+        <v>0.014388019899599425</v>
       </c>
     </row>
     <row r="72">
@@ -1775,7 +1778,7 @@
         <v>23</v>
       </c>
       <c r="D72" t="n">
-        <v>0.015160707654016836</v>
+        <v>0.014873896627109973</v>
       </c>
     </row>
     <row r="73">
@@ -1786,10 +1789,10 @@
         <v>105</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01562625404630022</v>
+        <v>0.015342174071644565</v>
       </c>
     </row>
     <row r="74">
@@ -1800,10 +1803,10 @@
         <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D74" t="n">
-        <v>0.01607005247381435</v>
+        <v>0.015790194190664852</v>
       </c>
     </row>
     <row r="75">
@@ -1814,10 +1817,10 @@
         <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>0.016489470724026956</v>
+        <v>0.01621535474742078</v>
       </c>
     </row>
     <row r="76">
@@ -1828,10 +1831,10 @@
         <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
-        <v>0.01688197076727571</v>
+        <v>0.016615134281926902</v>
       </c>
     </row>
     <row r="77">
@@ -1842,10 +1845,10 @@
         <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D77" t="n">
-        <v>0.01724513421447693</v>
+        <v>0.01698711687715873</v>
       </c>
     </row>
     <row r="78">
@@ -1856,10 +1859,10 @@
         <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D78" t="n">
-        <v>0.017576687055348733</v>
+        <v>0.017329016382335832</v>
       </c>
     </row>
     <row r="79">
@@ -1870,10 +1873,10 @@
         <v>113</v>
       </c>
       <c r="C79" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D79" t="n">
-        <v>0.017874523324380942</v>
+        <v>0.01763869975496274</v>
       </c>
     </row>
     <row r="80">
@@ -1884,10 +1887,10 @@
         <v>114</v>
       </c>
       <c r="C80" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D80" t="n">
-        <v>0.018136727350762924</v>
+        <v>0.017914209189121108</v>
       </c>
     </row>
     <row r="81">
@@ -1898,10 +1901,10 @@
         <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>0.018361594263842027</v>
+        <v>0.018153782709402183</v>
       </c>
     </row>
     <row r="82">
@@ -1912,10 +1915,10 @@
         <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D82" t="n">
-        <v>0.01854764844730096</v>
+        <v>0.018355872927743377</v>
       </c>
     </row>
     <row r="83">
@@ -1926,10 +1929,10 @@
         <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D83" t="n">
-        <v>0.018693659662711817</v>
+        <v>0.018519163683975354</v>
       </c>
     </row>
     <row r="84">
@@ -1940,10 +1943,10 @@
         <v>119</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D84" t="n">
-        <v>0.018798656596063387</v>
+        <v>0.018642584319812402</v>
       </c>
     </row>
     <row r="85">
@@ -1954,10 +1957,10 @@
         <v>121</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D85" t="n">
-        <v>0.018861937618593047</v>
+        <v>0.018725321369746833</v>
       </c>
     </row>
     <row r="86">
@@ -1968,10 +1971,10 @@
         <v>122</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D86" t="n">
-        <v>0.018883078595161397</v>
+        <v>0.01876682749026301</v>
       </c>
     </row>
     <row r="87">
@@ -1982,10 +1985,10 @@
         <v>123</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D87" t="n">
-        <v>0.01886193761859287</v>
+        <v>0.01876682749026301</v>
       </c>
     </row>
     <row r="88">
@@ -1996,10 +1999,10 @@
         <v>125</v>
       </c>
       <c r="C88" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>0.018798656596063397</v>
+        <v>0.018725321369746674</v>
       </c>
     </row>
     <row r="89">
@@ -2010,10 +2013,10 @@
         <v>126</v>
       </c>
       <c r="C89" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D89" t="n">
-        <v>0.018693659662711984</v>
+        <v>0.01864258431981239</v>
       </c>
     </row>
     <row r="90">
@@ -2024,10 +2027,10 @@
         <v>127</v>
       </c>
       <c r="C90" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D90" t="n">
-        <v>0.01854764844730096</v>
+        <v>0.018519163683975527</v>
       </c>
     </row>
     <row r="91">
@@ -2041,7 +2044,7 @@
         <v>11</v>
       </c>
       <c r="D91" t="n">
-        <v>0.018361594263841888</v>
+        <v>0.018355872927743377</v>
       </c>
     </row>
     <row r="92">
@@ -2055,7 +2058,7 @@
         <v>11</v>
       </c>
       <c r="D92" t="n">
-        <v>0.018136727350762896</v>
+        <v>0.018153782709402183</v>
       </c>
     </row>
     <row r="93">
@@ -2069,7 +2072,7 @@
         <v>11</v>
       </c>
       <c r="D93" t="n">
-        <v>0.01787452332438111</v>
+        <v>0.01791420918912094</v>
       </c>
     </row>
     <row r="94">
@@ -2080,10 +2083,10 @@
         <v>133</v>
       </c>
       <c r="C94" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D94" t="n">
-        <v>0.017576687055348733</v>
+        <v>0.017638699754962767</v>
       </c>
     </row>
     <row r="95">
@@ -2094,10 +2097,10 @@
         <v>134</v>
       </c>
       <c r="C95" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D95" t="n">
-        <v>0.017245134214476876</v>
+        <v>0.01732901638233597</v>
       </c>
     </row>
     <row r="96">
@@ -2108,10 +2111,10 @@
         <v>135</v>
       </c>
       <c r="C96" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D96" t="n">
-        <v>0.016881970767275767</v>
+        <v>0.01698711687715873</v>
       </c>
     </row>
     <row r="97">
@@ -2122,10 +2125,10 @@
         <v>137</v>
       </c>
       <c r="C97" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D97" t="n">
-        <v>0.016489470724026956</v>
+        <v>0.016615134281926902</v>
       </c>
     </row>
     <row r="98">
@@ -2136,10 +2139,10 @@
         <v>138</v>
       </c>
       <c r="C98" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D98" t="n">
-        <v>0.01607005247381435</v>
+        <v>0.016215354747420557</v>
       </c>
     </row>
     <row r="99">
@@ -2150,10 +2153,10 @@
         <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D99" t="n">
-        <v>0.015626254046300053</v>
+        <v>0.015790194190664936</v>
       </c>
     </row>
     <row r="100">
@@ -2164,10 +2167,10 @@
         <v>141</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D100" t="n">
-        <v>0.015160707654017058</v>
+        <v>0.015342174071644843</v>
       </c>
     </row>
     <row r="101">
@@ -2178,10 +2181,10 @@
         <v>142</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D101" t="n">
-        <v>0.014676113870492169</v>
+        <v>0.014873896627109862</v>
       </c>
     </row>
     <row r="102">
@@ -2192,10 +2195,10 @@
         <v>143</v>
       </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D102" t="n">
-        <v>0.014175215795704688</v>
+        <v>0.014388019899599425</v>
       </c>
     </row>
     <row r="103">
@@ -2206,10 +2209,10 @@
         <v>145</v>
       </c>
       <c r="C103" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D103" t="n">
-        <v>0.01366077355052564</v>
+        <v>0.013887232893715129</v>
       </c>
     </row>
     <row r="104">
@@ -2220,10 +2223,10 @@
         <v>146</v>
       </c>
       <c r="C104" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D104" t="n">
-        <v>0.013135539426153753</v>
+        <v>0.013374231179969054</v>
       </c>
     </row>
     <row r="105">
@@ -2234,10 +2237,10 @@
         <v>147</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D105" t="n">
-        <v>0.012602233993762813</v>
+        <v>0.012851693249620877</v>
       </c>
     </row>
     <row r="106">
@@ -2251,7 +2254,7 @@
         <v>11</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01206352345406203</v>
+        <v>0.012322257902281641</v>
       </c>
     </row>
     <row r="107">
@@ -2265,7 +2268,7 @@
         <v>11</v>
       </c>
       <c r="D107" t="n">
-        <v>0.011521998477022288</v>
+        <v>0.011788502922287947</v>
       </c>
     </row>
     <row r="108">
@@ -2279,7 +2282,7 @@
         <v>11</v>
       </c>
       <c r="D108" t="n">
-        <v>0.010980154749292481</v>
+        <v>0.01125292527060301</v>
       </c>
     </row>
     <row r="109">
@@ -2290,10 +2293,10 @@
         <v>153</v>
       </c>
       <c r="C109" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D109" t="n">
-        <v>0.010440375411636171</v>
+        <v>0.010717922986950512</v>
       </c>
     </row>
     <row r="110">
@@ -2304,10 +2307,10 @@
         <v>154</v>
       </c>
       <c r="C110" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D110" t="n">
-        <v>0.009904915531830205</v>
+        <v>0.010185778962807146</v>
       </c>
     </row>
     <row r="111">
@@ -2318,10 +2321,10 @@
         <v>155</v>
       </c>
       <c r="C111" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D111" t="n">
-        <v>0.009375888720689063</v>
+        <v>0.009658646710481944</v>
       </c>
     </row>
     <row r="112">
@@ -2335,7 +2338,7 @@
         <v>11</v>
       </c>
       <c r="D112" t="n">
-        <v>0.008855255961014386</v>
+        <v>0.009138538217574543</v>
       </c>
     </row>
     <row r="113">
@@ -2349,7 +2352,7 @@
         <v>11</v>
       </c>
       <c r="D113" t="n">
-        <v>0.008344816682026468</v>
+        <v>0.008627313940323456</v>
       </c>
     </row>
     <row r="114">
@@ -2363,7 +2366,7 @@
         <v>11</v>
       </c>
       <c r="D114" t="n">
-        <v>0.007846202075944164</v>
+        <v>0.008126674954427648</v>
       </c>
     </row>
     <row r="115">
@@ -2374,10 +2377,10 @@
         <v>161</v>
       </c>
       <c r="C115" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D115" t="n">
-        <v>0.007360870619459392</v>
+        <v>0.007638157248494537</v>
       </c>
     </row>
     <row r="116">
@@ -2388,10 +2391,10 @@
         <v>162</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D116" t="n">
-        <v>0.006890105731457097</v>
+        <v>0.007163128113875095</v>
       </c>
     </row>
     <row r="117">
@@ -2402,10 +2405,10 @@
         <v>163</v>
       </c>
       <c r="C117" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D117" t="n">
-        <v>0.0064350154699442386</v>
+        <v>0.006702784555806918</v>
       </c>
     </row>
     <row r="118">
@@ -2416,10 +2419,10 @@
         <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D118" t="n">
-        <v>0.005996534146116006</v>
+        <v>0.006258153624912388</v>
       </c>
     </row>
     <row r="119">
@@ -2430,10 +2433,10 @@
         <v>166</v>
       </c>
       <c r="C119" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D119" t="n">
-        <v>0.0055754257121434225</v>
+        <v>0.005830094545484554</v>
       </c>
     </row>
     <row r="120">
@@ -2444,10 +2447,10 @@
         <v>167</v>
       </c>
       <c r="C120" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D120" t="n">
-        <v>0.005172288761737587</v>
+        <v>0.005419302497937484</v>
       </c>
     </row>
     <row r="121">
@@ -2458,10 +2461,10 @@
         <v>169</v>
       </c>
       <c r="C121" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D121" t="n">
-        <v>0.004787562968970982</v>
+        <v>0.005026313897343926</v>
       </c>
     </row>
     <row r="122">
@@ -2472,10 +2475,10 @@
         <v>170</v>
       </c>
       <c r="C122" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D122" t="n">
-        <v>0.004421536781177182</v>
+        <v>0.0046515129983100145</v>
       </c>
     </row>
     <row r="123">
@@ -2486,10 +2489,10 @@
         <v>171</v>
       </c>
       <c r="C123" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D123" t="n">
-        <v>0.004074356175970038</v>
+        <v>0.004295139648408386</v>
       </c>
     </row>
     <row r="124">
@@ -2500,10 +2503,10 @@
         <v>173</v>
       </c>
       <c r="C124" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D124" t="n">
-        <v>0.003746034290295089</v>
+        <v>0.003957298007991987</v>
       </c>
     </row>
     <row r="125">
@@ -2514,10 +2517,10 @@
         <v>174</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D125" t="n">
-        <v>0.003436461730799263</v>
+        <v>0.0036379660531880575</v>
       </c>
     </row>
     <row r="126">
@@ -2528,10 +2531,10 @@
         <v>175</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D126" t="n">
-        <v>0.0031454173792980697</v>
+        <v>0.0033370056810835547</v>
       </c>
     </row>
     <row r="127">
@@ -2542,10 +2545,10 @@
         <v>177</v>
       </c>
       <c r="C127" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0028725795145188443</v>
+        <v>0.0030541732411913484</v>
       </c>
     </row>
     <row r="128">
@@ -2556,225 +2559,225 @@
         <v>178</v>
       </c>
       <c r="C128" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D128" t="n">
-        <v>0.00261753708109997</v>
+        <v>0.002789130324967217</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B129" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C129" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0023798009487685026</v>
+        <v>0.0025414546550541935</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B130" t="s">
         <v>181</v>
       </c>
       <c r="C130" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D130" t="n">
-        <v>0.0021588150181977087</v>
+        <v>0.0023106509276930483</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B131" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0019539670449252797</v>
+        <v>0.0020961614749889813</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B132" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C132" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0017645990684498746</v>
+        <v>0.0018973766280731517</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B133" t="s">
         <v>185</v>
       </c>
       <c r="C133" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0015900173498727115</v>
+        <v>0.0017136446772780915</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B134" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C134" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0014295017378235797</v>
+        <v>0.0015442813409155993</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B135" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C135" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D135" t="n">
-        <v>0.0012823143986088973</v>
+        <v>0.001388578669758526</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B136" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C136" t="s">
         <v>11</v>
       </c>
       <c r="D136" t="n">
-        <v>0.001147707862230436</v>
+        <v>0.0012458133296105456</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B137" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C137" t="s">
         <v>11</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0010249323509077934</v>
+        <v>0.0011152542191053237</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B138" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C138" t="s">
         <v>11</v>
       </c>
       <c r="D138" t="n">
-        <v>9.132423707729868E-4</v>
+        <v>9.961693939074933E-4</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B139" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C139" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D139" t="n">
-        <v>8.119025603279106E-4</v>
+        <v>8.878322815843278E-4</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B140" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C140" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D140" t="n">
-        <v>7.201928009306436E-4</v>
+        <v>7.895271834311036E-4</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B141" t="s">
         <v>196</v>
       </c>
       <c r="C141" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D141" t="n">
-        <v>6.374126049153057E-4</v>
+        <v>7.005540703561046E-4</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B142" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C142" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D142" t="n">
-        <v>5.628848059011935E-4</v>
+        <v>6.202326894772063E-4</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B143" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="C143" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D143" t="n">
-        <v>4.959585833917532E-4</v>
+        <v>5.479060063160513E-4</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B144" t="s">
         <v>200</v>
@@ -2783,49 +2786,49 @@
         <v>6</v>
       </c>
       <c r="D144" t="n">
-        <v>4.3601185991681054E-4</v>
+        <v>4.82943014384262E-4</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B145" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C145" t="s">
         <v>6</v>
       </c>
       <c r="D145" t="n">
-        <v>3.824531137760286E-4</v>
+        <v>4.24740949557632E-4</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B146" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C146" t="s">
         <v>6</v>
       </c>
       <c r="D146" t="n">
-        <v>3.3472265395979904E-4</v>
+        <v>3.7272695097251935E-4</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B147" t="s">
         <v>204</v>
       </c>
       <c r="C147" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D147" t="n">
-        <v>2.92293406144298E-4</v>
+        <v>3.263592133193956E-4</v>
       </c>
     </row>
     <row r="148">
@@ -2839,7 +2842,7 @@
         <v>6</v>
       </c>
       <c r="D148" t="n">
-        <v>2.5467125987688275E-4</v>
+        <v>2.851276774318526E-4</v>
       </c>
     </row>
     <row r="149">
@@ -2853,7 +2856,7 @@
         <v>6</v>
       </c>
       <c r="D149" t="n">
-        <v>2.2139502729944926E-4</v>
+        <v>2.485543070728921E-4</v>
       </c>
     </row>
     <row r="150">
@@ -2867,7 +2870,7 @@
         <v>6</v>
       </c>
       <c r="D150" t="n">
-        <v>1.9203606311700883E-4</v>
+        <v>2.1619299990756563E-4</v>
       </c>
     </row>
     <row r="151">
@@ -2878,10 +2881,10 @@
         <v>210</v>
       </c>
       <c r="C151" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D151" t="n">
-        <v>1.6619759412949005E-4</v>
+        <v>1.876291799340331E-4</v>
       </c>
     </row>
     <row r="152">
@@ -2892,10 +2895,10 @@
         <v>211</v>
       </c>
       <c r="C152" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D152" t="n">
-        <v>1.4351380462694846E-4</v>
+        <v>1.624791172377655E-4</v>
       </c>
     </row>
     <row r="153">
@@ -2906,10 +2909,10 @@
         <v>212</v>
       </c>
       <c r="C153" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D153" t="n">
-        <v>1.2364872142239065E-4</v>
+        <v>1.403890189497763E-4</v>
       </c>
     </row>
     <row r="154">
@@ -2920,10 +2923,10 @@
         <v>214</v>
       </c>
       <c r="C154" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D154" t="n">
-        <v>1.0629493937539696E-4</v>
+        <v>1.2103393284026867E-4</v>
       </c>
     </row>
     <row r="155">
@@ -2934,29 +2937,29 @@
         <v>215</v>
       </c>
       <c r="C155" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D155" t="n">
-        <v>9.117222505186369E-5</v>
+        <v>1.0411650217097301E-4</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
+        <v>213</v>
+      </c>
+      <c r="B156" t="s">
         <v>216</v>
       </c>
-      <c r="B156" t="s">
-        <v>217</v>
-      </c>
       <c r="C156" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D156" t="n">
-        <v>7.802603276866422E-5</v>
+        <v>8.936560736178727E-5</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B157" t="s">
         <v>218</v>
@@ -2965,12 +2968,12 @@
         <v>23</v>
       </c>
       <c r="D157" t="n">
-        <v>6.66259637765423E-5</v>
+        <v>7.653492679195325E-5</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B158" t="s">
         <v>219</v>
@@ -2979,26 +2982,26 @@
         <v>23</v>
       </c>
       <c r="D158" t="n">
-        <v>5.676419581900435E-5</v>
+        <v>6.540144573573232E-5</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>217</v>
+      </c>
+      <c r="B159" t="s">
         <v>220</v>
       </c>
-      <c r="B159" t="s">
-        <v>221</v>
-      </c>
       <c r="C159" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D159" t="n">
-        <v>4.825390683763851E-5</v>
+        <v>5.5763939100260244E-5</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B160" t="s">
         <v>222</v>
@@ -3007,12 +3010,12 @@
         <v>6</v>
       </c>
       <c r="D160" t="n">
-        <v>4.092771323297849E-5</v>
+        <v>4.744145035201822E-5</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B161" t="s">
         <v>223</v>
@@ -3021,133 +3024,147 @@
         <v>6</v>
       </c>
       <c r="D161" t="n">
-        <v>3.463613988169908E-5</v>
+        <v>4.027178584150283E-5</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
+        <v>221</v>
+      </c>
+      <c r="B162" t="s">
         <v>224</v>
       </c>
-      <c r="B162" t="s">
-        <v>225</v>
-      </c>
       <c r="C162" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D162" t="n">
-        <v>2.924613609298749E-5</v>
+        <v>3.411004070620922E-5</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B163" t="s">
         <v>226</v>
       </c>
       <c r="C163" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D163" t="n">
-        <v>2.4639648886750476E-5</v>
+        <v>2.882716968449623E-5</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B164" t="s">
         <v>227</v>
       </c>
       <c r="C164" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D164" t="n">
-        <v>2.0712262413304574E-5</v>
+        <v>2.430861353215745E-5</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
+        <v>225</v>
+      </c>
+      <c r="B165" t="s">
         <v>228</v>
       </c>
-      <c r="B165" t="s">
-        <v>229</v>
-      </c>
       <c r="C165" t="s">
         <v>6</v>
       </c>
       <c r="D165" t="n">
-        <v>1.7371910019377786E-5</v>
+        <v>2.04529893172828E-5</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B166" t="s">
         <v>230</v>
       </c>
       <c r="C166" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D166" t="n">
-        <v>1.4537663403318214E-5</v>
+        <v>1.717085068725874E-5</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B167" t="s">
         <v>231</v>
       </c>
       <c r="C167" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D167" t="n">
-        <v>1.2138601491805891E-5</v>
+        <v>1.4383522258392336E-5</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="s">
+        <v>229</v>
+      </c>
+      <c r="B168" t="s">
         <v>232</v>
       </c>
-      <c r="B168" t="s">
-        <v>233</v>
-      </c>
       <c r="C168" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D168" t="n">
-        <v>1.0112760104766496E-5</v>
+        <v>1.2022010572145841E-5</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B169" t="s">
         <v>234</v>
       </c>
       <c r="C169" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D169" t="n">
-        <v>8.40616214430677E-6</v>
+        <v>1.0025992586088788E-5</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B170" t="s">
         <v>235</v>
       </c>
       <c r="C170" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="D170" t="n">
-        <v>6.97192693372405E-6</v>
+        <v>8.34288141264879E-6</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="s">
+        <v>233</v>
+      </c>
+      <c r="B171" t="s">
+        <v>236</v>
+      </c>
+      <c r="C171" t="s">
+        <v>23</v>
+      </c>
+      <c r="D171" t="n">
+        <v>6.926967971821188E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now it works 100%
</commit_message>
<xml_diff>
--- a/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
+++ b/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="233">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,181 +26,502 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Angela Merkel</t>
-  </si>
-  <si>
-    <t>Politics and the Cthulu mythos</t>
+    <t>Lord Percy Percy</t>
+  </si>
+  <si>
+    <t>the English class system and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>flaunting foppish fashions in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> providing comic relief in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>James Dean</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
-    <t xml:space="preserve"> European politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Germany and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Dave Lee Roth</t>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Keith Richards</t>
   </si>
   <si>
     <t>Rock music and the Cthulu mythos</t>
   </si>
   <si>
-    <t>singing rock songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Elton John</t>
-  </si>
-  <si>
-    <t>Music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pop music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Love songs and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Savonarola</t>
-  </si>
-  <si>
-    <t>Florence and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Renaissance and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Chandler Bing</t>
-  </si>
-  <si>
-    <t>Friends and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>making sarcastic remarks in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Santa Claus</t>
-  </si>
-  <si>
-    <t>the North Pole and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christmas and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>delivering presents in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mary Poppins</t>
+    <t>playing rock music in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> playing rock guitar in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ridley Scott</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Special Effects and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>making fantasy movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> directing science fiction movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sarah Connor</t>
+  </si>
+  <si>
+    <t>The Terminator and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Post-Apocalypse and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>amassing weapons in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Chris Rock</t>
+  </si>
+  <si>
+    <t>Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Frank Sinatra</t>
+  </si>
+  <si>
+    <t>Easy Listening and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Rat Pack and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing middle-of-the-road songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Marie Curie</t>
+  </si>
+  <si>
+    <t>Physics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern science and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Chemistry and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Eric Cartman</t>
+  </si>
+  <si>
+    <t>South Park and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>executing morally appalling plans in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making racist jibes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Norman Bates</t>
+  </si>
+  <si>
+    <t>Psycho and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hitchcock movies and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Tony Montana</t>
+  </si>
+  <si>
+    <t>the Miami crime world and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a crime family in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> running an empire in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sheldon Cooper</t>
+  </si>
+  <si>
+    <t>The Big Bang Theory and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>studying science in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> collecting comic books in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>William Randolph Hearst</t>
+  </si>
+  <si>
+    <t>the Newspaper industry and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>running a media empire in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> publishing newspapers in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Michelangelo</t>
+  </si>
+  <si>
+    <t>Renaissance art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sculpture and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Painting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Marco Pierre White</t>
+  </si>
+  <si>
+    <t>Cooking and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jackson Pollock</t>
+  </si>
+  <si>
+    <t>Modern art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abstract art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Abstract painting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Novak Djokovic</t>
+  </si>
+  <si>
+    <t>Tennis and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>delivering forehand slams in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> winning tennis tournaments in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>The HamBurglar</t>
+  </si>
+  <si>
+    <t>McDonalds and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Hamburger industry and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>stealing hamburgers in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Janet Jackson</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Robert Mueller</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Law and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>chasing criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>George Harrison</t>
+  </si>
+  <si>
+    <t>The Beatles and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pop music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>playing guitar in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Brian Griffin</t>
+  </si>
+  <si>
+    <t>Family Guy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting liberal values in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ranting about conservatives in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>Basketball and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>playing basketball in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making dunk shots in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Nancy Drew</t>
   </si>
   <si>
     <t>Children's tales and the Dagon mythos</t>
   </si>
   <si>
-    <t>looking after children in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Dante Alighieri</t>
-  </si>
-  <si>
-    <t>Italian literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Italian poetry and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing poetry in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Christian Grey</t>
-  </si>
-  <si>
-    <t>Fifty Shades of Grey and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a multinational corporation in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> seducing women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Harvey Milk</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>campaigning for social causes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Emperor Constantine</t>
-  </si>
-  <si>
-    <t>Roman politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Ancient Rome and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running an empire in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Arya Stark</t>
-  </si>
-  <si>
-    <t>Game of Thrones and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Westeros and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>seeking revenge in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ivanka Trump</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Croesus</t>
-  </si>
-  <si>
-    <t>Lydia and the Cthulu mythos</t>
+    <t>solving mysteries in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Del Boy Trotter</t>
+  </si>
+  <si>
+    <t>Only Fools and Horses  and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  British comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British humour and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Scarlett Johansson</t>
+  </si>
+  <si>
+    <t>cross-dressing in women's clothes in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>David Hasselhoff</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baywatch and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Knight Rider and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Jerry Lewis</t>
+  </si>
+  <si>
+    <t>Comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Movies and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Kim Kardashian</t>
+  </si>
+  <si>
+    <t>Reality TV and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> flaunting buttocks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Leonard Hofstadter</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> obeying annoying rules in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Yoda</t>
+  </si>
+  <si>
+    <t>Star Wars and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>fighting for the resistance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> promoting mysticism in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Niccolò Paganini</t>
+  </si>
+  <si>
+    <t>Violin music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Classical music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>playing the violin in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stanley Kowalski</t>
+  </si>
+  <si>
+    <t>A Street Car Named Desire and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>moaning about women in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Xena</t>
+  </si>
+  <si>
+    <t>Ancient Greece and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>fighting for justice in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> defending the weak in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Peter Griffin</t>
+  </si>
+  <si>
+    <t>making silly decisions in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dan Quayle</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Right and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>campaigning for the senate in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sideshow Bob</t>
+  </si>
+  <si>
+    <t>The Simpsons and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>developing cunning plans in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Nick Fury</t>
+  </si>
+  <si>
+    <t>S.H.I.E.L.D. and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a clandestine spy organization in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Daniel Day-Lewis</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serious Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>performing serious acting in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Alexander the Great</t>
+  </si>
+  <si>
+    <t>War and the Cthulu mythos</t>
   </si>
   <si>
     <t xml:space="preserve"> the Ancient world and the Cthulu mythos</t>
   </si>
   <si>
-    <t>collecting treasures in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Lord Macbeth</t>
-  </si>
-  <si>
-    <t>British politics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British royalty and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Shakespeare and the Dagon mythos</t>
+    <t>building empires in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Katniss Everdeen</t>
+  </si>
+  <si>
+    <t>Science Fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hunger Games and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> spreading revolution in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>David Caruso</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CSI: Miami and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Police Procedurals and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Bruce Banner</t>
+  </si>
+  <si>
+    <t>Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>flying into a rage in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bursting out of shirts in Dagon-worshipping societies</t>
   </si>
   <si>
     <t>Che Guevara</t>
@@ -215,319 +536,172 @@
     <t xml:space="preserve"> Cuba and the Cthulu mythos</t>
   </si>
   <si>
-    <t>Jerry Maguire</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American sports and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American football and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>promoting greed in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Osama Bin Laden</t>
-  </si>
-  <si>
-    <t>Islamic Terrorism and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the War on Terror and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>plotting terrorist outrages in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Niccolò Paganini</t>
-  </si>
-  <si>
-    <t>Violin music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Classical music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>playing the violin in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Erik "Magneto" Lehnsherr</t>
-  </si>
-  <si>
-    <t>Marvel Comics and the Dagon mythos</t>
+    <t>Angelina Jolie</t>
+  </si>
+  <si>
+    <t>adopting children in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Leon Trotsky</t>
+  </si>
+  <si>
+    <t>Russian politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>wielding political power in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> promoting communism in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joseph Stalin</t>
+  </si>
+  <si>
+    <t>the Soviet Union and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Cold War and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a communist country in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Louis Pasteur</t>
+  </si>
+  <si>
+    <t>Science and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Chemistry and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>studying science in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Professor Charles Xavier</t>
   </si>
   <si>
     <t xml:space="preserve"> The X-Men and the Dagon mythos</t>
   </si>
   <si>
-    <t>devising evil schemes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Fagin</t>
-  </si>
-  <si>
-    <t>Oliver Twist and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Barbie</t>
-  </si>
-  <si>
-    <t>the Toy Industry and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>promoting hair products in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Monica Lewinsky</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Clinton Era and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>conducting illicit affairs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> causing political scandals in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Nigella Lawson</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Alan Sugar</t>
-  </si>
-  <si>
-    <t>British business and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>selling consumer goods in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Garry Kasparov</t>
-  </si>
-  <si>
-    <t>Chess and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing aggressive chess in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Staff Member</t>
-  </si>
-  <si>
-    <t>Research Area and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Research Activity in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Peter Jackson</t>
-  </si>
-  <si>
-    <t>The Lord of the Rings and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Hobbit and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>making fantasy movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Wolfgang Amadeus Mozart</t>
-  </si>
-  <si>
-    <t>Classical music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>composing classical music in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> playing the piano in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Larry Flynt</t>
-  </si>
-  <si>
-    <t>Hustler Magazine and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Soft pornography and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>publishing soft pornography in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Snake Plissken</t>
-  </si>
-  <si>
-    <t>Escape From New York and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Science Fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>going on commando missions in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tom Wolfe</t>
-  </si>
-  <si>
-    <t>Politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the News and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>writing about social problems in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tupac Shakur</t>
-  </si>
-  <si>
-    <t>Rap music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hip-Hop and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing rap songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Matt Drudge</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Marco Polo</t>
-  </si>
-  <si>
-    <t>the Age of Discovery and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>opening new markets in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> exploring foreign countries in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Whitney Houston</t>
-  </si>
-  <si>
-    <t>Pop Music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>John Merrick</t>
-  </si>
-  <si>
-    <t>Victorian England and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>hiding from the public in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> working in a freak show in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Linus Torvalds</t>
-  </si>
-  <si>
-    <t>Linux and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Operating Systems and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>developing open-source software in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Han Solo</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>piloting the Millenium Falcon in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> doing the Kessel run in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Angelina Jolie</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>adopting children in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joe Biden</t>
-  </si>
-  <si>
-    <t>the Left and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Democrats and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>plagiarizing political speeches in Cthulhu-worshipping societies</t>
+    <t>teaching young mutants in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> promoting diversity in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Mother Teresa</t>
+  </si>
+  <si>
+    <t>Calcutta and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> India and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Christianity and the Cthulu-Dagon mythos</t>
   </si>
   <si>
     <t>Ernest Hemingway</t>
   </si>
   <si>
+    <t>American literature and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing short stories in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing modern fiction in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Henry Miller</t>
+  </si>
+  <si>
     <t>American literature and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t>writing short stories in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing about manly pursuits in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jim Jones</t>
-  </si>
-  <si>
-    <t>Christian Fundamentalism and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running a religious cult in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> organizing mass suicides  in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Liz Lemon</t>
+    <t>writing erotic fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Luke Skywalker</t>
+  </si>
+  <si>
+    <t>fighting for the rebel alliance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> rescuing damsels in distress in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Doris Day</t>
+  </si>
+  <si>
+    <t>starring in romantic comedies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bane</t>
+  </si>
+  <si>
+    <t>DC Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gotham City and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>breaking heads in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Mickey Mouse</t>
+  </si>
+  <si>
+    <t>Walt Disney animation and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting movie violence in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in animated movies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Frodo Baggins</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hobbit and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>disposing of unwanted jewelry in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Alan Turing</t>
+  </si>
+  <si>
+    <t>Mathematics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Computers and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crypography and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Justin Timberlake</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tweeny music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>entertaining teenagers in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> singing to teenagers in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jenna Maroney</t>
   </si>
   <si>
     <t>30 Rock and the Dagon mythos</t>
@@ -536,193 +710,7 @@
     <t xml:space="preserve"> Television Production and the Dagon mythos</t>
   </si>
   <si>
-    <t>writing comedy in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bill Murray</t>
-  </si>
-  <si>
-    <t>American comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American culture and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in indy movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bruce Lee</t>
-  </si>
-  <si>
-    <t>Martial Arts and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Kung Fu and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>performing kung-fu moves in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Iggy Pop</t>
-  </si>
-  <si>
-    <t>Music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jazz and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blues music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Henry Kissinger</t>
-  </si>
-  <si>
-    <t>brokering peace deals in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Edmund Blackadder</t>
-  </si>
-  <si>
-    <t>the English class system and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>manipulating political pawns in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> climbing social ladders in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Donald Duck</t>
-  </si>
-  <si>
-    <t>Walt Disney animation and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>eating Peking duck in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> setting mousetraps in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Frank Zappa</t>
-  </si>
-  <si>
-    <t>Experimental music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing experimental songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing experimental songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Rain Man</t>
-  </si>
-  <si>
-    <t>Autism and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>counting tooth picks in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> counting cards in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jack Kerouac</t>
-  </si>
-  <si>
-    <t>the Beat generation and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American literature and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>writing beat fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>James Comey</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Law and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a bureaucracy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chasing criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Robin Hood</t>
-  </si>
-  <si>
-    <t>British legend and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British history and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sherwood Forest and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Spongebob Squarepants</t>
-  </si>
-  <si>
-    <t>Nickelodeon and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bikini Bottom and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>flipping hamburgers in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ray Charles</t>
-  </si>
-  <si>
-    <t>Pop Music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Boris Johnson</t>
-  </si>
-  <si>
-    <t>British politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the British Right the Conservative Party and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>making political gaffes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Xena</t>
-  </si>
-  <si>
-    <t>Ancient Greece and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for justice in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> defending the weak in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Hans Moleman</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Simpsons and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>getting run over by cars in Dagon-worshipping societies</t>
+    <t>singing pop songs in Dagon-worshipping societies</t>
   </si>
 </sst>
 </file>
@@ -798,7 +786,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>6.926967971821188E-6</v>
+        <v>7.110363806049832E-6</v>
       </c>
     </row>
     <row r="3">
@@ -812,7 +800,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>8.342881412648925E-6</v>
+        <v>8.601745231605532E-6</v>
       </c>
     </row>
     <row r="4">
@@ -826,7 +814,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0025992586088537E-5</v>
+        <v>1.0381804721807963E-5</v>
       </c>
     </row>
     <row r="5">
@@ -837,10 +825,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2022010572145957E-5</v>
+        <v>1.2501170060694193E-5</v>
       </c>
     </row>
     <row r="6">
@@ -848,284 +836,284 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>1.4383522258392336E-5</v>
+        <v>1.5018273112273788E-5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.717085068725874E-5</v>
+        <v>1.8000346273314564E-5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>2.0452989317283098E-5</v>
+        <v>2.152450876888403E-5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>2.430861353215688E-5</v>
+        <v>2.5678944288960617E-5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>2.8827169684496502E-5</v>
+        <v>3.0564170139829106E-5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>3.411004070620922E-5</v>
+        <v>3.629439649332022E-5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>4.027178584150283E-5</v>
+        <v>4.299897244410686E-5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>4.744145035201822E-5</v>
+        <v>5.082391341812632E-5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>5.576393910025932E-5</v>
+        <v>5.99335020069445E-5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>6.540144573573324E-5</v>
+        <v>7.051195153252572E-5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>7.653492679195325E-5</v>
+        <v>8.276511858166044E-5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D17" t="n">
-        <v>8.936560736178727E-5</v>
+        <v>9.692224740424178E-5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D18" t="n">
-        <v>1.0411650217097301E-4</v>
+        <v>1.132377254705277E-4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D19" t="n">
-        <v>1.2103393284026791E-4</v>
+        <v>1.3199282566522157E-4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D20" t="n">
-        <v>1.4038901894977706E-4</v>
+        <v>1.5349740660938087E-4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>1.624791172377655E-4</v>
+        <v>1.7809153850495418E-4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D22" t="n">
-        <v>1.876291799340331E-4</v>
+        <v>2.0614701776547058E-4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D23" t="n">
-        <v>2.1619299990756563E-4</v>
+        <v>2.3806872961709626E-4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D24" t="n">
-        <v>2.485543070728921E-4</v>
+        <v>2.7429581392686224E-4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>2.8512767743184655E-4</v>
+        <v>3.153025858523772E-4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
@@ -1134,12 +1122,12 @@
         <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>3.2635921331940166E-4</v>
+        <v>3.615991596344517E-4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
@@ -1148,7 +1136,7 @@
         <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>3.7272695097251935E-4</v>
+        <v>4.1373172110301766E-4</v>
       </c>
     </row>
     <row r="28">
@@ -1162,7 +1150,7 @@
         <v>6</v>
       </c>
       <c r="D28" t="n">
-        <v>4.24740949557632E-4</v>
+        <v>4.722823923817088E-4</v>
       </c>
     </row>
     <row r="29">
@@ -1176,7 +1164,7 @@
         <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>4.82943014384262E-4</v>
+        <v>5.378686310020353E-4</v>
       </c>
     </row>
     <row r="30">
@@ -1190,7 +1178,7 @@
         <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>5.479060063160461E-4</v>
+        <v>6.111421053237647E-4</v>
       </c>
     </row>
     <row r="31">
@@ -1201,10 +1189,10 @@
         <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D31" t="n">
-        <v>6.202326894772089E-4</v>
+        <v>6.927869889500763E-4</v>
       </c>
     </row>
     <row r="32">
@@ -1215,10 +1203,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D32" t="n">
-        <v>7.005540703561072E-4</v>
+        <v>7.835176188645508E-4</v>
       </c>
     </row>
     <row r="33">
@@ -1229,10 +1217,10 @@
         <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>7.895271834311036E-4</v>
+        <v>8.840754654305593E-4</v>
       </c>
     </row>
     <row r="34">
@@ -1243,10 +1231,10 @@
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D34" t="n">
-        <v>8.878322815843278E-4</v>
+        <v>9.952253672960145E-4</v>
       </c>
     </row>
     <row r="35">
@@ -1254,13 +1242,13 @@
         <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D35" t="n">
-        <v>9.961693939075107E-4</v>
+        <v>0.0011177509907283872</v>
       </c>
     </row>
     <row r="36">
@@ -1268,391 +1256,391 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0011152542191052942</v>
+        <v>0.0012524494810329852</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" t="s">
         <v>55</v>
       </c>
-      <c r="B37" t="s">
-        <v>56</v>
-      </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0012458133296105577</v>
+        <v>0.0014001252835105296</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>0.001388578669758526</v>
+        <v>0.0015615831228916691</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0015442813409155993</v>
+        <v>0.0017376201432910045</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="B40" t="s">
         <v>59</v>
       </c>
-      <c r="B40" t="s">
-        <v>60</v>
-      </c>
       <c r="C40" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0017136446772780915</v>
+        <v>0.0019290172253670652</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0018973766280731448</v>
+        <v>0.0021365295134174386</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0020961614749889883</v>
+        <v>0.002360876202382633</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" t="s">
         <v>63</v>
       </c>
-      <c r="B43" t="s">
-        <v>64</v>
-      </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0023106509276930483</v>
+        <v>0.0026027296529468474</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0025414546550541935</v>
+        <v>0.002862703921806018</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D45" t="n">
-        <v>0.002789130324967217</v>
+        <v>0.003141342813390579</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
         <v>67</v>
       </c>
-      <c r="B46" t="s">
-        <v>68</v>
-      </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0030541732411913276</v>
+        <v>0.0034391075784852496</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D47" t="n">
-        <v>0.003337005681083534</v>
+        <v>0.0037563644038760696</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D48" t="n">
-        <v>0.003637966053188099</v>
+        <v>0.004093371854887742</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
         <v>71</v>
       </c>
-      <c r="B49" t="s">
-        <v>72</v>
-      </c>
       <c r="C49" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D49" t="n">
-        <v>0.003957298007991987</v>
+        <v>0.00445026844901332</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D50" t="n">
-        <v>0.004295139648408386</v>
+        <v>0.00482706055324067</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
-        <v>0.004651512998309848</v>
+        <v>0.005223610809719337</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
         <v>75</v>
       </c>
-      <c r="B52" t="s">
-        <v>76</v>
-      </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>0.005026313897343981</v>
+        <v>0.005639627303529293</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>0.005419302497937595</v>
+        <v>0.006074653692131671</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.005830094545484554</v>
+        <v>0.0065280605181446405</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" t="s">
         <v>79</v>
       </c>
-      <c r="B55" t="s">
-        <v>80</v>
-      </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D55" t="n">
-        <v>0.006258153624912388</v>
+        <v>0.006999037925039586</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D56" t="n">
-        <v>0.006702784555806973</v>
+        <v>0.007486589988927483</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D57" t="n">
-        <v>0.007163128113875039</v>
+        <v>0.007989530868603212</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>82</v>
+      </c>
+      <c r="B58" t="s">
         <v>83</v>
       </c>
-      <c r="B58" t="s">
-        <v>84</v>
-      </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D58" t="n">
-        <v>0.007638157248494426</v>
+        <v>0.008506482960265571</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D59" t="n">
-        <v>0.00812667495442776</v>
+        <v>0.009035877222927313</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D60" t="n">
-        <v>0.008627313940323456</v>
+        <v>0.00957595581549242</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" t="s">
         <v>87</v>
       </c>
-      <c r="B61" t="s">
-        <v>88</v>
-      </c>
       <c r="C61" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D61" t="n">
-        <v>0.009138538217574543</v>
+        <v>0.010124777157069387</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D62" t="n">
-        <v>0.009658646710481888</v>
+        <v>0.010680223488663598</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D63" t="n">
-        <v>0.01018577896280709</v>
+        <v>0.011240010977377368</v>
       </c>
     </row>
     <row r="64">
@@ -1660,13 +1648,13 @@
         <v>90</v>
       </c>
       <c r="B64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>0.010717922986950623</v>
+        <v>0.011801702364261923</v>
       </c>
     </row>
     <row r="65">
@@ -1674,27 +1662,27 @@
         <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.01125292527060301</v>
+        <v>0.012362722114648728</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.011788502922287947</v>
+        <v>0.012920373985945977</v>
       </c>
     </row>
     <row r="67">
@@ -1702,13 +1690,13 @@
         <v>94</v>
       </c>
       <c r="B67" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D67" t="n">
-        <v>0.012322257902281752</v>
+        <v>0.013471860883380649</v>
       </c>
     </row>
     <row r="68">
@@ -1716,27 +1704,27 @@
         <v>94</v>
       </c>
       <c r="B68" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D68" t="n">
-        <v>0.012851693249620766</v>
+        <v>0.014014306829862544</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D69" t="n">
-        <v>0.013374231179969054</v>
+        <v>0.014544780833067594</v>
       </c>
     </row>
     <row r="70">
@@ -1744,209 +1732,209 @@
         <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70" t="n">
-        <v>0.013887232893715129</v>
+        <v>0.015060322391909187</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
       </c>
       <c r="D71" t="n">
-        <v>0.014388019899599425</v>
+        <v>0.015557968346771422</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>98</v>
+      </c>
+      <c r="B72" t="s">
         <v>101</v>
       </c>
-      <c r="B72" t="s">
-        <v>103</v>
-      </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="n">
-        <v>0.014873896627109973</v>
+        <v>0.016034780744138694</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>0.015342174071644565</v>
+        <v>0.01648787535747706</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" t="s">
         <v>104</v>
       </c>
-      <c r="B74" t="s">
-        <v>106</v>
-      </c>
       <c r="C74" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D74" t="n">
-        <v>0.015790194190664852</v>
+        <v>0.0169144504831423</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>0.01621535474742078</v>
+        <v>0.017311815613450854</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
         <v>107</v>
       </c>
-      <c r="B76" t="s">
-        <v>109</v>
-      </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
-        <v>0.016615134281926902</v>
+        <v>0.017677419579359144</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C77" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D77" t="n">
-        <v>0.01698711687715873</v>
+        <v>0.01800887775290233</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B78" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D78" t="n">
-        <v>0.017329016382335832</v>
+        <v>0.018303997904858524</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" t="s">
         <v>111</v>
       </c>
-      <c r="B79" t="s">
-        <v>113</v>
-      </c>
       <c r="C79" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D79" t="n">
-        <v>0.01763869975496274</v>
+        <v>0.0185608043261382</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D80" t="n">
-        <v>0.017914209189121108</v>
+        <v>0.018777559842025615</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C81" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>0.018153782709402183</v>
+        <v>0.018952785376332312</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" t="s">
         <v>115</v>
       </c>
-      <c r="B82" t="s">
-        <v>117</v>
-      </c>
       <c r="C82" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D82" t="n">
-        <v>0.018355872927743377</v>
+        <v>0.01908527675734257</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C83" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D83" t="n">
-        <v>0.018519163683975354</v>
+        <v>0.019174118498446628</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C84" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D84" t="n">
-        <v>0.018642584319812402</v>
+        <v>0.01921869433286312</v>
       </c>
     </row>
     <row r="85">
@@ -1954,102 +1942,102 @@
         <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C85" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D85" t="n">
-        <v>0.018725321369746833</v>
+        <v>0.019218694332863467</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B86" t="s">
         <v>122</v>
       </c>
       <c r="C86" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D86" t="n">
-        <v>0.01876682749026301</v>
+        <v>0.019174118498446455</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>121</v>
+      </c>
+      <c r="B87" t="s">
         <v>123</v>
       </c>
-      <c r="B87" t="s">
-        <v>124</v>
-      </c>
       <c r="C87" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>0.01876682749026301</v>
+        <v>0.019085276757342395</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C88" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>0.018725321369746674</v>
+        <v>0.018952785376332645</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B89" t="s">
         <v>126</v>
       </c>
       <c r="C89" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D89" t="n">
-        <v>0.01864258431981239</v>
+        <v>0.018777559842025462</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>125</v>
+      </c>
+      <c r="B90" t="s">
         <v>127</v>
       </c>
-      <c r="B90" t="s">
-        <v>128</v>
-      </c>
       <c r="C90" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D90" t="n">
-        <v>0.018519163683975527</v>
+        <v>0.01856080432613816</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B91" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C91" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D91" t="n">
-        <v>0.018355872927743377</v>
+        <v>0.018303997904858663</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B92" t="s">
         <v>130</v>
@@ -2058,26 +2046,26 @@
         <v>6</v>
       </c>
       <c r="D92" t="n">
-        <v>0.018153782709402183</v>
+        <v>0.018008877752902303</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>129</v>
+      </c>
+      <c r="B93" t="s">
         <v>131</v>
       </c>
-      <c r="B93" t="s">
-        <v>132</v>
-      </c>
       <c r="C93" t="s">
         <v>6</v>
       </c>
       <c r="D93" t="n">
-        <v>0.01791420918912094</v>
+        <v>0.01767741957935906</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B94" t="s">
         <v>133</v>
@@ -2086,12 +2074,12 @@
         <v>6</v>
       </c>
       <c r="D94" t="n">
-        <v>0.017638699754962767</v>
+        <v>0.017311815613450993</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B95" t="s">
         <v>134</v>
@@ -2100,96 +2088,96 @@
         <v>6</v>
       </c>
       <c r="D95" t="n">
-        <v>0.01732901638233597</v>
+        <v>0.016914450483142107</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>132</v>
+      </c>
+      <c r="B96" t="s">
         <v>135</v>
       </c>
-      <c r="B96" t="s">
-        <v>136</v>
-      </c>
       <c r="C96" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D96" t="n">
-        <v>0.01698711687715873</v>
+        <v>0.01648787535747709</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
         <v>137</v>
       </c>
       <c r="C97" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D97" t="n">
-        <v>0.016615134281926902</v>
+        <v>0.01603478074413886</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C98" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D98" t="n">
-        <v>0.016215354747420557</v>
+        <v>0.015557968346771256</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B99" t="s">
         <v>140</v>
       </c>
       <c r="C99" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D99" t="n">
-        <v>0.015790194190664936</v>
+        <v>0.015060322391909187</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B100" t="s">
         <v>141</v>
       </c>
       <c r="C100" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D100" t="n">
-        <v>0.015342174071644843</v>
+        <v>0.014544780833067483</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B101" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C101" t="s">
         <v>6</v>
       </c>
       <c r="D101" t="n">
-        <v>0.014873896627109862</v>
+        <v>0.014014306829862766</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B102" t="s">
         <v>144</v>
@@ -2198,12 +2186,12 @@
         <v>6</v>
       </c>
       <c r="D102" t="n">
-        <v>0.014388019899599425</v>
+        <v>0.013471860883380593</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B103" t="s">
         <v>145</v>
@@ -2212,152 +2200,152 @@
         <v>6</v>
       </c>
       <c r="D103" t="n">
-        <v>0.013887232893715129</v>
+        <v>0.01292037398594581</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B104" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
       </c>
       <c r="D104" t="n">
-        <v>0.013374231179969054</v>
+        <v>0.012362722114648783</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B105" t="s">
         <v>148</v>
       </c>
       <c r="C105" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D105" t="n">
-        <v>0.012851693249620877</v>
+        <v>0.011801702364262034</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B106" t="s">
         <v>149</v>
       </c>
       <c r="C106" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D106" t="n">
-        <v>0.012322257902281641</v>
+        <v>0.011240010977377202</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B107" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C107" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D107" t="n">
-        <v>0.011788502922287947</v>
+        <v>0.010680223488663765</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
         <v>152</v>
       </c>
       <c r="C108" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D108" t="n">
-        <v>0.01125292527060301</v>
+        <v>0.010124777157069387</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B109" t="s">
         <v>153</v>
       </c>
       <c r="C109" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D109" t="n">
-        <v>0.010717922986950512</v>
+        <v>0.009575955815492254</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B110" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C110" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D110" t="n">
-        <v>0.010185778962807146</v>
+        <v>0.009035877222927424</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B111" t="s">
         <v>156</v>
       </c>
       <c r="C111" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D111" t="n">
-        <v>0.009658646710481944</v>
+        <v>0.008506482960265516</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B112" t="s">
         <v>157</v>
       </c>
       <c r="C112" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D112" t="n">
-        <v>0.009138538217574543</v>
+        <v>0.007989530868603156</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B113" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="n">
-        <v>0.008627313940323456</v>
+        <v>0.007486589988927594</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B114" t="s">
         <v>160</v>
@@ -2366,12 +2354,12 @@
         <v>6</v>
       </c>
       <c r="D114" t="n">
-        <v>0.008126674954427648</v>
+        <v>0.00699903792503942</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B115" t="s">
         <v>161</v>
@@ -2380,68 +2368,68 @@
         <v>6</v>
       </c>
       <c r="D115" t="n">
-        <v>0.007638157248494537</v>
+        <v>0.006528060518144696</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B116" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C116" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D116" t="n">
-        <v>0.007163128113875095</v>
+        <v>0.006074653692131837</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B117" t="s">
         <v>164</v>
       </c>
       <c r="C117" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D117" t="n">
-        <v>0.006702784555806918</v>
+        <v>0.005639627303529127</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B118" t="s">
         <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D118" t="n">
-        <v>0.006258153624912388</v>
+        <v>0.005223610809719337</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="B119" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C119" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D119" t="n">
-        <v>0.005830094545484554</v>
+        <v>0.004827060553240781</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B120" t="s">
         <v>168</v>
@@ -2450,12 +2438,12 @@
         <v>6</v>
       </c>
       <c r="D120" t="n">
-        <v>0.005419302497937484</v>
+        <v>0.0044502684490132435</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B121" t="s">
         <v>169</v>
@@ -2464,203 +2452,203 @@
         <v>6</v>
       </c>
       <c r="D121" t="n">
-        <v>0.005026313897343926</v>
+        <v>0.004093371854887708</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C122" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D122" t="n">
-        <v>0.0046515129983100145</v>
+        <v>0.003756364403876139</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B123" t="s">
         <v>172</v>
       </c>
       <c r="C123" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D123" t="n">
-        <v>0.004295139648408386</v>
+        <v>0.003439107578485194</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B124" t="s">
         <v>173</v>
       </c>
       <c r="C124" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D124" t="n">
-        <v>0.003957298007991987</v>
+        <v>0.003141342813390565</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B125" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C125" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D125" t="n">
-        <v>0.0036379660531880575</v>
+        <v>0.0028627039218060493</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B126" t="s">
         <v>176</v>
       </c>
       <c r="C126" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D126" t="n">
-        <v>0.0033370056810835547</v>
+        <v>0.0026027296529468787</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B127" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C127" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0030541732411913484</v>
+        <v>0.0023608762023825704</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="B128" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C128" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D128" t="n">
-        <v>0.002789130324967217</v>
+        <v>0.0021365295134174907</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B129" t="s">
         <v>180</v>
       </c>
       <c r="C129" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0025414546550541935</v>
+        <v>0.0019290172253670183</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B130" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C130" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D130" t="n">
-        <v>0.0023106509276930483</v>
+        <v>0.0017376201432909993</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B131" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C131" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D131" t="n">
-        <v>0.0020961614749889813</v>
+        <v>0.001561583122891676</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B132" t="s">
         <v>184</v>
       </c>
       <c r="C132" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0018973766280731517</v>
+        <v>0.0014001252835105296</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B133" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C133" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0017136446772780915</v>
+        <v>0.0012524494810329783</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B134" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C134" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0015442813409155993</v>
+        <v>0.0011177509907284184</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B135" t="s">
         <v>188</v>
       </c>
       <c r="C135" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D135" t="n">
-        <v>0.001388578669758526</v>
+        <v>9.952253672959877E-4</v>
       </c>
     </row>
     <row r="136">
@@ -2671,10 +2659,10 @@
         <v>190</v>
       </c>
       <c r="C136" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D136" t="n">
-        <v>0.0012458133296105456</v>
+        <v>8.84075465430555E-4</v>
       </c>
     </row>
     <row r="137">
@@ -2685,10 +2673,10 @@
         <v>191</v>
       </c>
       <c r="C137" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D137" t="n">
-        <v>0.0011152542191053237</v>
+        <v>7.835176188645612E-4</v>
       </c>
     </row>
     <row r="138">
@@ -2699,10 +2687,10 @@
         <v>192</v>
       </c>
       <c r="C138" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D138" t="n">
-        <v>9.961693939074933E-4</v>
+        <v>6.927869889500719E-4</v>
       </c>
     </row>
     <row r="139">
@@ -2713,10 +2701,10 @@
         <v>194</v>
       </c>
       <c r="C139" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D139" t="n">
-        <v>8.878322815843278E-4</v>
+        <v>6.111421053237587E-4</v>
       </c>
     </row>
     <row r="140">
@@ -2727,10 +2715,10 @@
         <v>195</v>
       </c>
       <c r="C140" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D140" t="n">
-        <v>7.895271834311036E-4</v>
+        <v>5.378686310020453E-4</v>
       </c>
     </row>
     <row r="141">
@@ -2741,10 +2729,10 @@
         <v>196</v>
       </c>
       <c r="C141" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D141" t="n">
-        <v>7.005540703561046E-4</v>
+        <v>4.722823923817062E-4</v>
       </c>
     </row>
     <row r="142">
@@ -2755,10 +2743,10 @@
         <v>198</v>
       </c>
       <c r="C142" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D142" t="n">
-        <v>6.202326894772063E-4</v>
+        <v>4.137317211030103E-4</v>
       </c>
     </row>
     <row r="143">
@@ -2769,10 +2757,10 @@
         <v>199</v>
       </c>
       <c r="C143" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D143" t="n">
-        <v>5.479060063160513E-4</v>
+        <v>3.615991596344569E-4</v>
       </c>
     </row>
     <row r="144">
@@ -2783,10 +2771,10 @@
         <v>200</v>
       </c>
       <c r="C144" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D144" t="n">
-        <v>4.82943014384262E-4</v>
+        <v>3.153025858523761E-4</v>
       </c>
     </row>
     <row r="145">
@@ -2797,10 +2785,10 @@
         <v>202</v>
       </c>
       <c r="C145" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D145" t="n">
-        <v>4.24740949557632E-4</v>
+        <v>2.742958139268581E-4</v>
       </c>
     </row>
     <row r="146">
@@ -2811,66 +2799,66 @@
         <v>203</v>
       </c>
       <c r="C146" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D146" t="n">
-        <v>3.7272695097251935E-4</v>
+        <v>2.380687296170993E-4</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B147" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C147" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D147" t="n">
-        <v>3.263592133193956E-4</v>
+        <v>2.0614701776547036E-4</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B148" t="s">
         <v>206</v>
       </c>
       <c r="C148" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D148" t="n">
-        <v>2.851276774318526E-4</v>
+        <v>1.7809153850495136E-4</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B149" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C149" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D149" t="n">
-        <v>2.485543070728921E-4</v>
+        <v>1.5349740660938293E-4</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="B150" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C150" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D150" t="n">
-        <v>2.1619299990756563E-4</v>
+        <v>1.319928256652195E-4</v>
       </c>
     </row>
     <row r="151">
@@ -2878,13 +2866,13 @@
         <v>209</v>
       </c>
       <c r="B151" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C151" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D151" t="n">
-        <v>1.876291799340331E-4</v>
+        <v>1.132377254705277E-4</v>
       </c>
     </row>
     <row r="152">
@@ -2892,27 +2880,27 @@
         <v>209</v>
       </c>
       <c r="B152" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C152" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D152" t="n">
-        <v>1.624791172377655E-4</v>
+        <v>9.692224740424427E-5</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="B153" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C153" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D153" t="n">
-        <v>1.403890189497763E-4</v>
+        <v>8.276511858165795E-5</v>
       </c>
     </row>
     <row r="154">
@@ -2920,13 +2908,13 @@
         <v>213</v>
       </c>
       <c r="B154" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C154" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D154" t="n">
-        <v>1.2103393284026867E-4</v>
+        <v>7.051195153252572E-5</v>
       </c>
     </row>
     <row r="155">
@@ -2934,27 +2922,27 @@
         <v>213</v>
       </c>
       <c r="B155" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C155" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D155" t="n">
-        <v>1.0411650217097301E-4</v>
+        <v>5.9933502006945315E-5</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="B156" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C156" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D156" t="n">
-        <v>8.936560736178727E-5</v>
+        <v>5.082391341812632E-5</v>
       </c>
     </row>
     <row r="157">
@@ -2962,13 +2950,13 @@
         <v>217</v>
       </c>
       <c r="B157" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C157" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D157" t="n">
-        <v>7.653492679195325E-5</v>
+        <v>4.2998972444106045E-5</v>
       </c>
     </row>
     <row r="158">
@@ -2976,27 +2964,27 @@
         <v>217</v>
       </c>
       <c r="B158" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C158" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D158" t="n">
-        <v>6.540144573573232E-5</v>
+        <v>3.629439649332106E-5</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="B159" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C159" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D159" t="n">
-        <v>5.5763939100260244E-5</v>
+        <v>3.056417013982854E-5</v>
       </c>
     </row>
     <row r="160">
@@ -3004,13 +2992,13 @@
         <v>221</v>
       </c>
       <c r="B160" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C160" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D160" t="n">
-        <v>4.744145035201822E-5</v>
+        <v>2.5678944288960346E-5</v>
       </c>
     </row>
     <row r="161">
@@ -3018,27 +3006,27 @@
         <v>221</v>
       </c>
       <c r="B161" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C161" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D161" t="n">
-        <v>4.027178584150283E-5</v>
+        <v>2.152450876888403E-5</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="B162" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C162" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D162" t="n">
-        <v>3.411004070620922E-5</v>
+        <v>1.800034627331478E-5</v>
       </c>
     </row>
     <row r="163">
@@ -3046,13 +3034,13 @@
         <v>225</v>
       </c>
       <c r="B163" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C163" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D163" t="n">
-        <v>2.882716968449623E-5</v>
+        <v>1.5018273112273788E-5</v>
       </c>
     </row>
     <row r="164">
@@ -3060,27 +3048,27 @@
         <v>225</v>
       </c>
       <c r="B164" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C164" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D164" t="n">
-        <v>2.430861353215745E-5</v>
+        <v>1.2501170060693976E-5</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="B165" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C165" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D165" t="n">
-        <v>2.04529893172828E-5</v>
+        <v>1.0381804721808085E-5</v>
       </c>
     </row>
     <row r="166">
@@ -3088,13 +3076,13 @@
         <v>229</v>
       </c>
       <c r="B166" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C166" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D166" t="n">
-        <v>1.717085068725874E-5</v>
+        <v>8.601745231605526E-6</v>
       </c>
     </row>
     <row r="167">
@@ -3102,69 +3090,13 @@
         <v>229</v>
       </c>
       <c r="B167" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C167" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D167" t="n">
-        <v>1.4383522258392336E-5</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="s">
-        <v>229</v>
-      </c>
-      <c r="B168" t="s">
-        <v>232</v>
-      </c>
-      <c r="C168" t="s">
-        <v>22</v>
-      </c>
-      <c r="D168" t="n">
-        <v>1.2022010572145841E-5</v>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="s">
-        <v>233</v>
-      </c>
-      <c r="B169" t="s">
-        <v>234</v>
-      </c>
-      <c r="C169" t="s">
-        <v>22</v>
-      </c>
-      <c r="D169" t="n">
-        <v>1.0025992586088788E-5</v>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="s">
-        <v>233</v>
-      </c>
-      <c r="B170" t="s">
-        <v>235</v>
-      </c>
-      <c r="C170" t="s">
-        <v>22</v>
-      </c>
-      <c r="D170" t="n">
-        <v>8.34288141264879E-6</v>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="s">
-        <v>233</v>
-      </c>
-      <c r="B171" t="s">
-        <v>236</v>
-      </c>
-      <c r="C171" t="s">
-        <v>22</v>
-      </c>
-      <c r="D171" t="n">
-        <v>6.926967971821188E-6</v>
+        <v>7.1103638060497165E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed project input files for each preference sheet
</commit_message>
<xml_diff>
--- a/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
+++ b/Test_Sets/Project_Sets/src/main/resources/projects120.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="227">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,691 +26,673 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Lord Percy Percy</t>
+    <t>Brad Pitt</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Thomas Jefferson</t>
+  </si>
+  <si>
+    <t>American history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>campaigning for democracy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Buffy Summers</t>
+  </si>
+  <si>
+    <t>Horror and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>hunting demons in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> hunting monsters in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stewie Griffin</t>
+  </si>
+  <si>
+    <t>Family Guy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>plotting against family members in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pioneering new technologies in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Clint Eastwood</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in action movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Francis Crick</t>
+  </si>
+  <si>
+    <t>Biology and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DNA and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Double Helix and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Groucho Marx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Marx Brothers and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in madcap comedies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Rupert Murdoch</t>
+  </si>
+  <si>
+    <t>the Newspaper industry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Fox News and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a media empire in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Lord Macbeth</t>
+  </si>
+  <si>
+    <t>British politics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British royalty and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shakespeare and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Orson Welles</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serious Acting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Superman</t>
+  </si>
+  <si>
+    <t>DC Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Metropolis and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Daily Planet and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Larry Flynt</t>
+  </si>
+  <si>
+    <t>Hustler Magazine and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Soft pornography and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>publishing soft pornography in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Britney Spears</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tweeny music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>flirting with rednecks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Steven Spielberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Special Effects and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> producing Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ray Charles</t>
+  </si>
+  <si>
+    <t>Pop Music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Inspector Jacques Clouseau</t>
+  </si>
+  <si>
+    <t>the Gendarmerie and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>solving mysteries in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Federico Fellini</t>
+  </si>
+  <si>
+    <t>Italian Neo-realism and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making new wave movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making Italian movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>James Comey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Law and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>running a bureaucracy in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Elmer Fudd</t>
+  </si>
+  <si>
+    <t>Looney Tunes and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Warner Bros animation and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>hunting rabbits in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Stephen Colbert</t>
+  </si>
+  <si>
+    <t>Comedy Central and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting conservative values in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sun Tzu</t>
+  </si>
+  <si>
+    <t>The Art of War and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ancient military history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>developing military strategies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Monica Lewinsky</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Clinton Era and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>conducting illicit affairs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Arthur Conan Doyle</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing mystery stories in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Norma Desmond</t>
+  </si>
+  <si>
+    <t>Sunset Boulevard and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>clinging to past dreams in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dominique Strauss-Kahn</t>
+  </si>
+  <si>
+    <t>French politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>throwing sex parties in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> planning orgies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Sarah Connor</t>
+  </si>
+  <si>
+    <t>The Terminator and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Post-Apocalypse and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>amassing weapons in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dante Alighieri</t>
+  </si>
+  <si>
+    <t>Italian literature and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Italian poetry and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing poetry in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jane Goodall</t>
+  </si>
+  <si>
+    <t>Anthropology and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>living amongst apes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Michael Moore</t>
+  </si>
+  <si>
+    <t>Documentaries and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Left and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making provocative documentaries in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Mad Max Rockatansky</t>
+  </si>
+  <si>
+    <t>the Post-Apocalypse and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Action movies and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>avenging loved ones in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Tony Robbins</t>
+  </si>
+  <si>
+    <t>Neuro-Linguistic Programming and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Self-Help and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Self-Improvement and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Tina Turner</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing rock songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> gyrating hips in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Darth Vader</t>
+  </si>
+  <si>
+    <t>Star Wars and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Dark Side and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting the Dark Side in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ernest Hemingway</t>
+  </si>
+  <si>
+    <t>American literature and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing short stories in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing modern fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Kent Brockman</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Simpsons and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>reading the news in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bob Dylan</t>
+  </si>
+  <si>
+    <t>Folk music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Protest songs and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing protest songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Miles Davis</t>
+  </si>
+  <si>
+    <t>Cool Jazz and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jazz and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>playing jazz saxophone in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ryan Reynolds</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making dumb comedies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Matt Groening</t>
+  </si>
+  <si>
+    <t>The Simpsons and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Springfield and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing comedy in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Russell Brand</t>
+  </si>
+  <si>
+    <t>British comedy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British humour and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Movies and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Henry Miller</t>
+  </si>
+  <si>
+    <t>writing erotic fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Henry James</t>
+  </si>
+  <si>
+    <t>American literature and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing modern fiction in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Peter Jackson</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hobbit and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making fantasy movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Raymond Chandler</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing detective fiction in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Daniel Craig</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> James Bond and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> starring in indy movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> playing James Bond in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Adam Smith</t>
+  </si>
+  <si>
+    <t>Capitalism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting capitalism in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Matt "Daredevil" Murdock</t>
+  </si>
+  <si>
+    <t>Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>maintaining a secret identity in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pursuing criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Anne Boleyn</t>
+  </si>
+  <si>
+    <t>Politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British royalty and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Gerard Manley Hopkins</t>
+  </si>
+  <si>
+    <t>Poetry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sprung Rhyme and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing modern poetry in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>writing modern fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Princess Leia Organa</t>
+  </si>
+  <si>
+    <t>leading the rebel alliance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> smuggling military plans in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Law and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a bureaucracy in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> chasing criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>John Constantine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Horror and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hellraiser and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>smoking Silk Cut cigarettes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joan Rivers</t>
+  </si>
+  <si>
+    <t>Comedy and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>insulting celebrities in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> doing stand-up in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Al Bundy</t>
+  </si>
+  <si>
+    <t>Family life and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>watching TV in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Mark Zuckerberg</t>
+  </si>
+  <si>
+    <t>Facebook and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Technology and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Software and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Michelle Obama</t>
+  </si>
+  <si>
+    <t>the Left and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Democrats and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting feminism in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Philip Marlowe</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Lt. George Colthurst St Barleigh</t>
   </si>
   <si>
     <t>the English class system and the Dagon mythos</t>
   </si>
   <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>flaunting foppish fashions in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> providing comic relief in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>James Dean</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Keith Richards</t>
-  </si>
-  <si>
-    <t>Rock music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing rock music in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> playing rock guitar in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ridley Scott</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Special Effects and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>making fantasy movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> directing science fiction movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sarah Connor</t>
-  </si>
-  <si>
-    <t>The Terminator and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Post-Apocalypse and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>amassing weapons in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Chris Rock</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Frank Sinatra</t>
-  </si>
-  <si>
-    <t>Easy Listening and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Rat Pack and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing middle-of-the-road songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Marie Curie</t>
-  </si>
-  <si>
-    <t>Physics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Modern science and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Chemistry and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Eric Cartman</t>
-  </si>
-  <si>
-    <t>South Park and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>executing morally appalling plans in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making racist jibes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Norman Bates</t>
-  </si>
-  <si>
-    <t>Psycho and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hitchcock movies and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tony Montana</t>
-  </si>
-  <si>
-    <t>the Miami crime world and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a crime family in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> running an empire in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sheldon Cooper</t>
-  </si>
-  <si>
-    <t>The Big Bang Theory and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>studying science in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> collecting comic books in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>William Randolph Hearst</t>
-  </si>
-  <si>
-    <t>the Newspaper industry and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running a media empire in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> publishing newspapers in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Michelangelo</t>
-  </si>
-  <si>
-    <t>Renaissance art and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sculpture and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Painting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Marco Pierre White</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jackson Pollock</t>
-  </si>
-  <si>
-    <t>Modern art and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Abstract art and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Abstract painting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Novak Djokovic</t>
-  </si>
-  <si>
-    <t>Tennis and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>delivering forehand slams in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> winning tennis tournaments in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>The HamBurglar</t>
-  </si>
-  <si>
-    <t>McDonalds and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Hamburger industry and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>stealing hamburgers in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Janet Jackson</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Robert Mueller</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Law and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>chasing criminals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>George Harrison</t>
-  </si>
-  <si>
-    <t>The Beatles and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Pop music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>playing guitar in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Brian Griffin</t>
-  </si>
-  <si>
-    <t>Family Guy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>promoting liberal values in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ranting about conservatives in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Michael Jordan</t>
-  </si>
-  <si>
-    <t>Basketball and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing basketball in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making dunk shots in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Nancy Drew</t>
-  </si>
-  <si>
-    <t>Children's tales and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>solving mysteries in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Del Boy Trotter</t>
-  </si>
-  <si>
-    <t>Only Fools and Horses  and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  British comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British humour and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Scarlett Johansson</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Hasselhoff</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Baywatch and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Knight Rider and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jerry Lewis</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Movies and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Kim Kardashian</t>
-  </si>
-  <si>
-    <t>Reality TV and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> flaunting buttocks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Leonard Hofstadter</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> obeying annoying rules in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Yoda</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for the resistance in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> promoting mysticism in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Niccolò Paganini</t>
-  </si>
-  <si>
-    <t>Violin music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Classical music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing the violin in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Stanley Kowalski</t>
-  </si>
-  <si>
-    <t>A Street Car Named Desire and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>moaning about women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Xena</t>
-  </si>
-  <si>
-    <t>Ancient Greece and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for justice in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> defending the weak in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Peter Griffin</t>
-  </si>
-  <si>
-    <t>making silly decisions in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Dan Quayle</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Right and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>campaigning for the senate in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sideshow Bob</t>
-  </si>
-  <si>
-    <t>The Simpsons and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Springfield and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>developing cunning plans in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Nick Fury</t>
-  </si>
-  <si>
-    <t>S.H.I.E.L.D. and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Marvel Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a clandestine spy organization in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Daniel Day-Lewis</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Serious Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>performing serious acting in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Alexander the Great</t>
-  </si>
-  <si>
-    <t>War and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Ancient world and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>building empires in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Katniss Everdeen</t>
-  </si>
-  <si>
-    <t>Science Fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Hunger Games and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> spreading revolution in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Caruso</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CSI: Miami and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Police Procedurals and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Bruce Banner</t>
-  </si>
-  <si>
-    <t>Marvel Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>flying into a rage in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bursting out of shirts in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Che Guevara</t>
-  </si>
-  <si>
-    <t>Cuban politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Cuban revolution and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cuba and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Angelina Jolie</t>
-  </si>
-  <si>
-    <t>adopting children in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in Hollywood movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Leon Trotsky</t>
-  </si>
-  <si>
-    <t>Russian politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>wielding political power in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> promoting communism in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joseph Stalin</t>
-  </si>
-  <si>
-    <t>the Soviet Union and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Cold War and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a communist country in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Louis Pasteur</t>
-  </si>
-  <si>
-    <t>Science and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chemistry and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>studying science in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Professor Charles Xavier</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The X-Men and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>teaching young mutants in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> promoting diversity in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mother Teresa</t>
-  </si>
-  <si>
-    <t>Calcutta and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> India and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Christianity and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Ernest Hemingway</t>
-  </si>
-  <si>
-    <t>American literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing short stories in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing modern fiction in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Henry Miller</t>
-  </si>
-  <si>
-    <t>American literature and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>writing erotic fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Luke Skywalker</t>
-  </si>
-  <si>
-    <t>fighting for the rebel alliance in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rescuing damsels in distress in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Doris Day</t>
-  </si>
-  <si>
-    <t>starring in romantic comedies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bane</t>
-  </si>
-  <si>
-    <t>DC Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gotham City and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>breaking heads in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mickey Mouse</t>
-  </si>
-  <si>
-    <t>Walt Disney animation and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>promoting movie violence in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in animated movies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Frodo Baggins</t>
-  </si>
-  <si>
-    <t>The Lord of the Rings and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Hobbit and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>disposing of unwanted jewelry in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Alan Turing</t>
-  </si>
-  <si>
-    <t>Mathematics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Computers and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Crypography and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Justin Timberlake</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tweeny music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>entertaining teenagers in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> singing to teenagers in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Jenna Maroney</t>
-  </si>
-  <si>
-    <t>30 Rock and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Television Production and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing pop songs in Dagon-worshipping societies</t>
+    <t>providing comic relief in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dr. Henry Jekyll</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>suppressing violent urges in Dagon-worshipping societies</t>
   </si>
 </sst>
 </file>
@@ -786,7 +768,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>7.110363806049832E-6</v>
+        <v>7.30370196938962E-6</v>
       </c>
     </row>
     <row r="3">
@@ -800,7 +782,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>8.601745231605532E-6</v>
+        <v>8.876736087824355E-6</v>
       </c>
     </row>
     <row r="4">
@@ -814,7 +796,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>1.0381804721807963E-5</v>
+        <v>1.0762290101346865E-5</v>
       </c>
     </row>
     <row r="5">
@@ -828,7 +810,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>1.2501170060694193E-5</v>
+        <v>1.3016589298255957E-5</v>
       </c>
     </row>
     <row r="6">
@@ -842,7 +824,7 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>1.5018273112273788E-5</v>
+        <v>1.570474290888732E-5</v>
       </c>
     </row>
     <row r="7">
@@ -856,7 +838,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>1.8000346273314564E-5</v>
+        <v>1.8901905250990556E-5</v>
       </c>
     </row>
     <row r="8">
@@ -867,10 +849,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8" t="n">
-        <v>2.152450876888403E-5</v>
+        <v>2.2694543634126807E-5</v>
       </c>
     </row>
     <row r="9">
@@ -878,13 +860,13 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D9" t="n">
-        <v>2.5678944288960617E-5</v>
+        <v>2.7181814693938135E-5</v>
       </c>
     </row>
     <row r="10">
@@ -892,186 +874,186 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" t="n">
-        <v>3.0564170139829106E-5</v>
+        <v>3.247704914124936E-5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D11" t="n">
-        <v>3.629439649332022E-5</v>
+        <v>3.87093428827954E-5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D12" t="n">
-        <v>4.299897244410686E-5</v>
+        <v>4.60252500795423E-5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D13" t="n">
-        <v>5.082391341812632E-5</v>
+        <v>5.459057094030391E-5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>5.99335020069445E-5</v>
+        <v>6.459222389495822E-5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>7.051195153252572E-5</v>
+        <v>7.624018825416409E-5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>8.276511858166044E-5</v>
+        <v>8.976949955242982E-5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>9.692224740424178E-5</v>
+        <v>1.0544227551229871E-4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>1.132377254705277E-4</v>
+        <v>1.2354974599637593E-4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>30</v>
       </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>1.3199282566522157E-4</v>
+        <v>1.4441425548297586E-4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>1.5349740660938087E-4</v>
+        <v>1.683912015788061E-4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>1.7809153850495418E-4</v>
+        <v>1.9587086795381506E-4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
       <c r="C22" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D22" t="n">
-        <v>2.0614701776547058E-4</v>
+        <v>2.2728010495225875E-4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
@@ -1080,12 +1062,12 @@
         <v>11</v>
       </c>
       <c r="D23" t="n">
-        <v>2.3806872961709626E-4</v>
+        <v>2.630838061214145E-4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
@@ -1094,152 +1076,152 @@
         <v>11</v>
       </c>
       <c r="D24" t="n">
-        <v>2.7429581392686224E-4</v>
+        <v>3.037861241430128E-4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D25" t="n">
-        <v>3.153025858523772E-4</v>
+        <v>3.4993136530722495E-4</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D26" t="n">
-        <v>3.615991596344517E-4</v>
+        <v>4.02104497903788E-4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D27" t="n">
-        <v>4.1373172110301766E-4</v>
+        <v>4.6093120689932226E-4</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D28" t="n">
-        <v>4.722823923817088E-4</v>
+        <v>5.270774252151217E-4</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D29" t="n">
-        <v>5.378686310020353E-4</v>
+        <v>6.012482710063822E-4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D30" t="n">
-        <v>6.111421053237647E-4</v>
+        <v>6.841863207692096E-4</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
-        <v>6.927869889500763E-4</v>
+        <v>7.76669150047463E-4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D32" t="n">
-        <v>7.835176188645508E-4</v>
+        <v>8.79506077158098E-4</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D33" t="n">
-        <v>8.840754654305593E-4</v>
+        <v>9.935340508521332E-4</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D34" t="n">
-        <v>9.952253672960145E-4</v>
+        <v>0.0011196126303103055</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
@@ -1248,12 +1230,12 @@
         <v>6</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0011177509907283872</v>
+        <v>0.0012586180154336869</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
@@ -1262,26 +1244,26 @@
         <v>6</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0012524494810329852</v>
+        <v>0.0014114360970849255</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
       <c r="C37" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0014001252835105296</v>
+        <v>0.0015789545107691774</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>56</v>
@@ -1290,12 +1272,12 @@
         <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0015615831228916691</v>
+        <v>0.001762053693176736</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
         <v>57</v>
@@ -1304,49 +1286,49 @@
         <v>11</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0017376201432910045</v>
+        <v>0.001961596958920715</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
-        <v>59</v>
-      </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0019290172253670652</v>
+        <v>0.002178419634536185</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
         <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0021365295134174386</v>
+        <v>0.0024133173081108336</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D42" t="n">
-        <v>0.002360876202382633</v>
+        <v>0.0026670332754893146</v>
       </c>
     </row>
     <row r="43">
@@ -1357,10 +1339,10 @@
         <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0026027296529468474</v>
+        <v>0.0029402452874599284</v>
       </c>
     </row>
     <row r="44">
@@ -1371,10 +1353,10 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D44" t="n">
-        <v>0.002862703921806018</v>
+        <v>0.003233551726241537</v>
       </c>
     </row>
     <row r="45">
@@ -1385,10 +1367,10 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D45" t="n">
-        <v>0.003141342813390579</v>
+        <v>0.00354745736345137</v>
       </c>
     </row>
     <row r="46">
@@ -1399,10 +1381,10 @@
         <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D46" t="n">
-        <v>0.0034391075784852496</v>
+        <v>0.0038823588749923588</v>
       </c>
     </row>
     <row r="47">
@@ -1413,10 +1395,10 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D47" t="n">
-        <v>0.0037563644038760696</v>
+        <v>0.004238530310342929</v>
       </c>
     </row>
     <row r="48">
@@ -1427,10 +1409,10 @@
         <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D48" t="n">
-        <v>0.004093371854887742</v>
+        <v>0.004616108733958235</v>
       </c>
     </row>
     <row r="49">
@@ -1444,7 +1426,7 @@
         <v>11</v>
       </c>
       <c r="D49" t="n">
-        <v>0.00445026844901332</v>
+        <v>0.005015080274237915</v>
       </c>
     </row>
     <row r="50">
@@ -1458,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="D50" t="n">
-        <v>0.00482706055324067</v>
+        <v>0.005435266830137231</v>
       </c>
     </row>
     <row r="51">
@@ -1472,7 +1454,7 @@
         <v>11</v>
       </c>
       <c r="D51" t="n">
-        <v>0.005223610809719337</v>
+        <v>0.00587631369639785</v>
       </c>
     </row>
     <row r="52">
@@ -1486,7 +1468,7 @@
         <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>0.005639627303529293</v>
+        <v>0.006337678374936095</v>
       </c>
     </row>
     <row r="53">
@@ -1500,7 +1482,7 @@
         <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>0.006074653692131671</v>
+        <v>0.006818620841611611</v>
       </c>
     </row>
     <row r="54">
@@ -1514,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.0065280605181446405</v>
+        <v>0.007318195534039673</v>
       </c>
     </row>
     <row r="55">
@@ -1525,10 +1507,10 @@
         <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D55" t="n">
-        <v>0.006999037925039586</v>
+        <v>0.00783524531680635</v>
       </c>
     </row>
     <row r="56">
@@ -1539,10 +1521,10 @@
         <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D56" t="n">
-        <v>0.007486589988927483</v>
+        <v>0.008368397665311667</v>
       </c>
     </row>
     <row r="57">
@@ -1553,10 +1535,10 @@
         <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D57" t="n">
-        <v>0.007989530868603212</v>
+        <v>0.008916063288275877</v>
       </c>
     </row>
     <row r="58">
@@ -1567,10 +1549,10 @@
         <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D58" t="n">
-        <v>0.008506482960265571</v>
+        <v>0.009476437381783609</v>
       </c>
     </row>
     <row r="59">
@@ -1581,10 +1563,10 @@
         <v>84</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D59" t="n">
-        <v>0.009035877222927313</v>
+        <v>0.010047503674802893</v>
       </c>
     </row>
     <row r="60">
@@ -1595,10 +1577,10 @@
         <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D60" t="n">
-        <v>0.00957595581549242</v>
+        <v>0.010627041387692548</v>
       </c>
     </row>
     <row r="61">
@@ -1609,10 +1591,10 @@
         <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D61" t="n">
-        <v>0.010124777157069387</v>
+        <v>0.011212635181869823</v>
       </c>
     </row>
     <row r="62">
@@ -1623,10 +1605,10 @@
         <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D62" t="n">
-        <v>0.010680223488663598</v>
+        <v>0.011801688131175325</v>
       </c>
     </row>
     <row r="63">
@@ -1637,10 +1619,10 @@
         <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D63" t="n">
-        <v>0.011240010977377368</v>
+        <v>0.012391437694338592</v>
       </c>
     </row>
     <row r="64">
@@ -1654,7 +1636,7 @@
         <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>0.011801702364261923</v>
+        <v>0.012978974614322847</v>
       </c>
     </row>
     <row r="65">
@@ -1668,7 +1650,7 @@
         <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.012362722114648728</v>
+        <v>0.013561264615188862</v>
       </c>
     </row>
     <row r="66">
@@ -1682,7 +1664,7 @@
         <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.012920373985945977</v>
+        <v>0.014135172711703392</v>
       </c>
     </row>
     <row r="67">
@@ -1693,10 +1675,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>0.013471860883380649</v>
+        <v>0.014697489892400273</v>
       </c>
     </row>
     <row r="68">
@@ -1707,71 +1689,71 @@
         <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>0.014014306829862544</v>
+        <v>0.015244961884468555</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B69" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D69" t="n">
-        <v>0.014544780833067594</v>
+        <v>0.01577431965996251</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B70" t="s">
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D70" t="n">
-        <v>0.015060322391909187</v>
+        <v>0.016282311298634555</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B71" t="s">
         <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D71" t="n">
-        <v>0.015557968346771422</v>
+        <v>0.016765734784380926</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
       </c>
       <c r="D72" t="n">
-        <v>0.016034780744138694</v>
+        <v>0.01722147128091328</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
         <v>103</v>
@@ -1780,12 +1762,12 @@
         <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>0.01648787535747706</v>
+        <v>0.01764651840879153</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B74" t="s">
         <v>104</v>
@@ -1794,96 +1776,96 @@
         <v>6</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0169144504831423</v>
+        <v>0.018038023031183903</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C75" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D75" t="n">
-        <v>0.017311815613450854</v>
+        <v>0.018393313050183074</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B76" t="s">
         <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D76" t="n">
-        <v>0.017677419579359144</v>
+        <v>0.01870992771967983</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" t="s">
         <v>108</v>
       </c>
-      <c r="B77" t="s">
-        <v>109</v>
-      </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D77" t="n">
-        <v>0.01800887775290233</v>
+        <v>0.01898564599475981</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B78" t="s">
         <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D78" t="n">
-        <v>0.018303997904858524</v>
+        <v>0.019218512461317033</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B79" t="s">
         <v>111</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0185608043261382</v>
+        <v>0.019406860422715493</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>109</v>
+      </c>
+      <c r="B80" t="s">
         <v>112</v>
       </c>
-      <c r="B80" t="s">
-        <v>113</v>
-      </c>
       <c r="C80" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D80" t="n">
-        <v>0.018777559842025615</v>
+        <v>0.019549331762337203</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B81" t="s">
         <v>114</v>
@@ -1892,12 +1874,12 @@
         <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>0.018952785376332312</v>
+        <v>0.0196448932509484</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B82" t="s">
         <v>115</v>
@@ -1906,7 +1888,7 @@
         <v>11</v>
       </c>
       <c r="D82" t="n">
-        <v>0.01908527675734257</v>
+        <v>0.01969284902499017</v>
       </c>
     </row>
     <row r="83">
@@ -1917,10 +1899,10 @@
         <v>117</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D83" t="n">
-        <v>0.019174118498446628</v>
+        <v>0.01969284902499017</v>
       </c>
     </row>
     <row r="84">
@@ -1931,150 +1913,150 @@
         <v>118</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D84" t="n">
-        <v>0.01921869433286312</v>
+        <v>0.01964489325094804</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" t="s">
         <v>119</v>
       </c>
-      <c r="B85" t="s">
-        <v>120</v>
-      </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D85" t="n">
-        <v>0.019218694332863467</v>
+        <v>0.019549331762337384</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>120</v>
+      </c>
+      <c r="B86" t="s">
         <v>121</v>
       </c>
-      <c r="B86" t="s">
-        <v>122</v>
-      </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D86" t="n">
-        <v>0.019174118498446455</v>
+        <v>0.019406860422715673</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C87" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D87" t="n">
-        <v>0.019085276757342395</v>
+        <v>0.01921851246131666</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B88" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D88" t="n">
-        <v>0.018952785376332645</v>
+        <v>0.01898564599475984</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>124</v>
+      </c>
+      <c r="B89" t="s">
         <v>125</v>
       </c>
-      <c r="B89" t="s">
-        <v>126</v>
-      </c>
       <c r="C89" t="s">
         <v>11</v>
       </c>
       <c r="D89" t="n">
-        <v>0.018777559842025462</v>
+        <v>0.01870992771968004</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B90" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C90" t="s">
         <v>11</v>
       </c>
       <c r="D90" t="n">
-        <v>0.01856080432613816</v>
+        <v>0.018393313050183213</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B91" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91" t="n">
-        <v>0.018303997904858663</v>
+        <v>0.018038023031183903</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>128</v>
+      </c>
+      <c r="B92" t="s">
         <v>129</v>
       </c>
-      <c r="B92" t="s">
-        <v>130</v>
-      </c>
       <c r="C92" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D92" t="n">
-        <v>0.018008877752902303</v>
+        <v>0.017646518408791195</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B93" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C93" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D93" t="n">
-        <v>0.01767741957935906</v>
+        <v>0.017221471280913392</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B94" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C94" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D94" t="n">
-        <v>0.017311815613450993</v>
+        <v>0.016765734784381148</v>
       </c>
     </row>
     <row r="95">
@@ -2082,13 +2064,13 @@
         <v>132</v>
       </c>
       <c r="B95" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C95" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D95" t="n">
-        <v>0.016914450483142107</v>
+        <v>0.016282311298634222</v>
       </c>
     </row>
     <row r="96">
@@ -2096,209 +2078,209 @@
         <v>132</v>
       </c>
       <c r="B96" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C96" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D96" t="n">
-        <v>0.01648787535747709</v>
+        <v>0.015774319659962455</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B97" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C97" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D97" t="n">
-        <v>0.01603478074413886</v>
+        <v>0.015244961884468722</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B98" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D98" t="n">
-        <v>0.015557968346771256</v>
+        <v>0.014697489892400495</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>136</v>
+      </c>
+      <c r="B99" t="s">
         <v>138</v>
       </c>
-      <c r="B99" t="s">
-        <v>140</v>
-      </c>
       <c r="C99" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D99" t="n">
-        <v>0.015060322391909187</v>
+        <v>0.014135172711703392</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B100" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C100" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D100" t="n">
-        <v>0.014544780833067483</v>
+        <v>0.013561264615188529</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B101" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C101" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D101" t="n">
-        <v>0.014014306829862766</v>
+        <v>0.012978974614323069</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>140</v>
+      </c>
+      <c r="B102" t="s">
         <v>142</v>
       </c>
-      <c r="B102" t="s">
-        <v>144</v>
-      </c>
       <c r="C102" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D102" t="n">
-        <v>0.013471860883380593</v>
+        <v>0.012391437694338703</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B103" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C103" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D103" t="n">
-        <v>0.01292037398594581</v>
+        <v>0.011801688131175048</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B104" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C104" t="s">
         <v>6</v>
       </c>
       <c r="D104" t="n">
-        <v>0.012362722114648783</v>
+        <v>0.011212635181869879</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
+        <v>144</v>
+      </c>
+      <c r="B105" t="s">
         <v>146</v>
       </c>
-      <c r="B105" t="s">
-        <v>148</v>
-      </c>
       <c r="C105" t="s">
         <v>6</v>
       </c>
       <c r="D105" t="n">
-        <v>0.011801702364262034</v>
+        <v>0.010627041387692715</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B106" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C106" t="s">
         <v>6</v>
       </c>
       <c r="D106" t="n">
-        <v>0.011240010977377202</v>
+        <v>0.010047503674802949</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B107" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C107" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D107" t="n">
-        <v>0.010680223488663765</v>
+        <v>0.009476437381783609</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
+        <v>148</v>
+      </c>
+      <c r="B108" t="s">
         <v>150</v>
       </c>
-      <c r="B108" t="s">
-        <v>152</v>
-      </c>
       <c r="C108" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D108" t="n">
-        <v>0.010124777157069387</v>
+        <v>0.008916063288275822</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B109" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C109" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D109" t="n">
-        <v>0.009575955815492254</v>
+        <v>0.008368397665311722</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C110" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D110" t="n">
-        <v>0.009035877222927424</v>
+        <v>0.00783524531680635</v>
       </c>
     </row>
     <row r="111">
@@ -2306,13 +2288,13 @@
         <v>154</v>
       </c>
       <c r="B111" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C111" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D111" t="n">
-        <v>0.008506482960265516</v>
+        <v>0.007318195534039562</v>
       </c>
     </row>
     <row r="112">
@@ -2320,27 +2302,27 @@
         <v>154</v>
       </c>
       <c r="B112" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C112" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D112" t="n">
-        <v>0.007989530868603156</v>
+        <v>0.006818620841611389</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B113" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C113" t="s">
         <v>6</v>
       </c>
       <c r="D113" t="n">
-        <v>0.007486589988927594</v>
+        <v>0.0063376783749362064</v>
       </c>
     </row>
     <row r="114">
@@ -2348,13 +2330,13 @@
         <v>158</v>
       </c>
       <c r="B114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C114" t="s">
         <v>6</v>
       </c>
       <c r="D114" t="n">
-        <v>0.00699903792503942</v>
+        <v>0.005876313696398072</v>
       </c>
     </row>
     <row r="115">
@@ -2362,27 +2344,27 @@
         <v>158</v>
       </c>
       <c r="B115" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C115" t="s">
         <v>6</v>
       </c>
       <c r="D115" t="n">
-        <v>0.006528060518144696</v>
+        <v>0.005435266830137231</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B116" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C116" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D116" t="n">
-        <v>0.006074653692131837</v>
+        <v>0.005015080274237693</v>
       </c>
     </row>
     <row r="117">
@@ -2390,139 +2372,139 @@
         <v>162</v>
       </c>
       <c r="B117" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C117" t="s">
         <v>11</v>
       </c>
       <c r="D117" t="n">
-        <v>0.005639627303529127</v>
+        <v>0.004616108733958457</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B118" t="s">
         <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D118" t="n">
-        <v>0.005223610809719337</v>
+        <v>0.004238530310342929</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="s">
+        <v>164</v>
+      </c>
+      <c r="B119" t="s">
         <v>166</v>
       </c>
-      <c r="B119" t="s">
-        <v>167</v>
-      </c>
       <c r="C119" t="s">
         <v>6</v>
       </c>
       <c r="D119" t="n">
-        <v>0.004827060553240781</v>
+        <v>0.0038823588749922963</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B120" t="s">
         <v>168</v>
       </c>
       <c r="C120" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D120" t="n">
-        <v>0.0044502684490132435</v>
+        <v>0.0035474573634513597</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
         <v>169</v>
       </c>
       <c r="C121" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D121" t="n">
-        <v>0.004093371854887708</v>
+        <v>0.0032335517262415923</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
+        <v>167</v>
+      </c>
+      <c r="B122" t="s">
         <v>170</v>
       </c>
-      <c r="B122" t="s">
-        <v>171</v>
-      </c>
       <c r="C122" t="s">
         <v>11</v>
       </c>
       <c r="D122" t="n">
-        <v>0.003756364403876139</v>
+        <v>0.002940245287459946</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B123" t="s">
         <v>172</v>
       </c>
       <c r="C123" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D123" t="n">
-        <v>0.003439107578485194</v>
+        <v>0.0026670332754893146</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B124" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C124" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D124" t="n">
-        <v>0.003141342813390565</v>
+        <v>0.002413317308110785</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B125" t="s">
         <v>175</v>
       </c>
       <c r="C125" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D125" t="n">
-        <v>0.0028627039218060493</v>
+        <v>0.002178419634536223</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B126" t="s">
         <v>176</v>
       </c>
       <c r="C126" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D126" t="n">
-        <v>0.0026027296529468787</v>
+        <v>0.0019615969589207253</v>
       </c>
     </row>
     <row r="127">
@@ -2533,10 +2515,10 @@
         <v>178</v>
       </c>
       <c r="C127" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D127" t="n">
-        <v>0.0023608762023825704</v>
+        <v>0.0017620536931767083</v>
       </c>
     </row>
     <row r="128">
@@ -2547,71 +2529,71 @@
         <v>179</v>
       </c>
       <c r="C128" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D128" t="n">
-        <v>0.0021365295134174907</v>
+        <v>0.0015789545107691722</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="B129" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C129" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D129" t="n">
-        <v>0.0019290172253670183</v>
+        <v>0.001411436097084948</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B130" t="s">
         <v>182</v>
       </c>
       <c r="C130" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D130" t="n">
-        <v>0.0017376201432909993</v>
+        <v>0.0012586180154336973</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B131" t="s">
         <v>183</v>
       </c>
       <c r="C131" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D131" t="n">
-        <v>0.001561583122891676</v>
+        <v>0.0011196126303103055</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="B132" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C132" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D132" t="n">
-        <v>0.0014001252835105296</v>
+        <v>9.935340508521158E-4</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B133" t="s">
         <v>186</v>
@@ -2620,12 +2602,12 @@
         <v>11</v>
       </c>
       <c r="D133" t="n">
-        <v>0.0012524494810329783</v>
+        <v>8.79506077158111E-4</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B134" t="s">
         <v>187</v>
@@ -2634,63 +2616,63 @@
         <v>11</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0011177509907284184</v>
+        <v>7.766691500474673E-4</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B135" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C135" t="s">
         <v>11</v>
       </c>
       <c r="D135" t="n">
-        <v>9.952253672959877E-4</v>
+        <v>6.841863207691975E-4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B136" t="s">
         <v>190</v>
       </c>
       <c r="C136" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D136" t="n">
-        <v>8.84075465430555E-4</v>
+        <v>6.012482710063887E-4</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B137" t="s">
         <v>191</v>
       </c>
       <c r="C137" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D137" t="n">
-        <v>7.835176188645612E-4</v>
+        <v>5.270774252151204E-4</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="B138" t="s">
         <v>192</v>
       </c>
       <c r="C138" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D138" t="n">
-        <v>6.927869889500719E-4</v>
+        <v>4.609312068993292E-4</v>
       </c>
     </row>
     <row r="139">
@@ -2701,10 +2683,10 @@
         <v>194</v>
       </c>
       <c r="C139" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D139" t="n">
-        <v>6.111421053237587E-4</v>
+        <v>4.02104497903788E-4</v>
       </c>
     </row>
     <row r="140">
@@ -2715,388 +2697,332 @@
         <v>195</v>
       </c>
       <c r="C140" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D140" t="n">
-        <v>5.378686310020453E-4</v>
+        <v>3.499313653072219E-4</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="s">
-        <v>193</v>
+        <v>74</v>
       </c>
       <c r="B141" t="s">
         <v>196</v>
       </c>
       <c r="C141" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="D141" t="n">
-        <v>4.722823923817062E-4</v>
+        <v>3.037861241430126E-4</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="s">
+        <v>74</v>
+      </c>
+      <c r="B142" t="s">
         <v>197</v>
       </c>
-      <c r="B142" t="s">
-        <v>198</v>
-      </c>
       <c r="C142" t="s">
         <v>11</v>
       </c>
       <c r="D142" t="n">
-        <v>4.137317211030103E-4</v>
+        <v>2.630838061214178E-4</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>197</v>
+        <v>74</v>
       </c>
       <c r="B143" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C143" t="s">
         <v>11</v>
       </c>
       <c r="D143" t="n">
-        <v>3.615991596344569E-4</v>
+        <v>2.2728010495225355E-4</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B144" t="s">
         <v>200</v>
       </c>
       <c r="C144" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D144" t="n">
-        <v>3.153025858523761E-4</v>
+        <v>1.9587086795381462E-4</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="s">
+        <v>199</v>
+      </c>
+      <c r="B145" t="s">
         <v>201</v>
       </c>
-      <c r="B145" t="s">
-        <v>202</v>
-      </c>
       <c r="C145" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D145" t="n">
-        <v>2.742958139268581E-4</v>
+        <v>1.6839120157881033E-4</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B146" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C146" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D146" t="n">
-        <v>2.380687296170993E-4</v>
+        <v>1.4441425548297727E-4</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="s">
+        <v>203</v>
+      </c>
+      <c r="B147" t="s">
         <v>204</v>
       </c>
-      <c r="B147" t="s">
-        <v>205</v>
-      </c>
       <c r="C147" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D147" t="n">
-        <v>2.0614701776547036E-4</v>
+        <v>1.2354974599637593E-4</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B148" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C148" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D148" t="n">
-        <v>1.7809153850495136E-4</v>
+        <v>1.0544227551229795E-4</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B149" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C149" t="s">
         <v>11</v>
       </c>
       <c r="D149" t="n">
-        <v>1.5349740660938293E-4</v>
+        <v>8.976949955243058E-5</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B150" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C150" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D150" t="n">
-        <v>1.319928256652195E-4</v>
+        <v>7.624018825416409E-5</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="s">
+        <v>207</v>
+      </c>
+      <c r="B151" t="s">
         <v>209</v>
       </c>
-      <c r="B151" t="s">
-        <v>211</v>
-      </c>
       <c r="C151" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D151" t="n">
-        <v>1.132377254705277E-4</v>
+        <v>6.459222389495751E-5</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B152" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C152" t="s">
         <v>6</v>
       </c>
       <c r="D152" t="n">
-        <v>9.692224740424427E-5</v>
+        <v>5.459057094030369E-5</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B153" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C153" t="s">
         <v>6</v>
       </c>
       <c r="D153" t="n">
-        <v>8.276511858165795E-5</v>
+        <v>4.602525007954322E-5</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="s">
+        <v>210</v>
+      </c>
+      <c r="B154" t="s">
         <v>213</v>
       </c>
-      <c r="B154" t="s">
-        <v>215</v>
-      </c>
       <c r="C154" t="s">
         <v>6</v>
       </c>
       <c r="D154" t="n">
-        <v>7.051195153252572E-5</v>
+        <v>3.87093428827954E-5</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B155" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C155" t="s">
         <v>6</v>
       </c>
       <c r="D155" t="n">
-        <v>5.9933502006945315E-5</v>
+        <v>3.247704914124936E-5</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B156" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C156" t="s">
         <v>6</v>
       </c>
       <c r="D156" t="n">
-        <v>5.082391341812632E-5</v>
+        <v>2.7181814693937457E-5</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="s">
+        <v>214</v>
+      </c>
+      <c r="B157" t="s">
         <v>217</v>
       </c>
-      <c r="B157" t="s">
-        <v>219</v>
-      </c>
       <c r="C157" t="s">
         <v>6</v>
       </c>
       <c r="D157" t="n">
-        <v>4.2998972444106045E-5</v>
+        <v>2.269454363412743E-5</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B158" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C158" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D158" t="n">
-        <v>3.629439649332106E-5</v>
+        <v>1.890190525099061E-5</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="s">
+        <v>220</v>
+      </c>
+      <c r="B159" t="s">
         <v>221</v>
       </c>
-      <c r="B159" t="s">
-        <v>222</v>
-      </c>
       <c r="C159" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D159" t="n">
-        <v>3.056417013982854E-5</v>
+        <v>1.5704742908886885E-5</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B160" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C160" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D160" t="n">
-        <v>2.5678944288960346E-5</v>
+        <v>1.3016589298256052E-5</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B161" t="s">
         <v>224</v>
       </c>
       <c r="C161" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D161" t="n">
-        <v>2.152450876888403E-5</v>
+        <v>1.0762290101347034E-5</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
+        <v>223</v>
+      </c>
+      <c r="B162" t="s">
         <v>225</v>
       </c>
-      <c r="B162" t="s">
-        <v>226</v>
-      </c>
       <c r="C162" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D162" t="n">
-        <v>1.800034627331478E-5</v>
+        <v>8.876736087824524E-6</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B163" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C163" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D163" t="n">
-        <v>1.5018273112273788E-5</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="s">
-        <v>225</v>
-      </c>
-      <c r="B164" t="s">
-        <v>228</v>
-      </c>
-      <c r="C164" t="s">
-        <v>11</v>
-      </c>
-      <c r="D164" t="n">
-        <v>1.2501170060693976E-5</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="s">
-        <v>229</v>
-      </c>
-      <c r="B165" t="s">
-        <v>230</v>
-      </c>
-      <c r="C165" t="s">
-        <v>6</v>
-      </c>
-      <c r="D165" t="n">
-        <v>1.0381804721808085E-5</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="s">
-        <v>229</v>
-      </c>
-      <c r="B166" t="s">
-        <v>231</v>
-      </c>
-      <c r="C166" t="s">
-        <v>6</v>
-      </c>
-      <c r="D166" t="n">
-        <v>8.601745231605526E-6</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="s">
-        <v>229</v>
-      </c>
-      <c r="B167" t="s">
-        <v>232</v>
-      </c>
-      <c r="C167" t="s">
-        <v>6</v>
-      </c>
-      <c r="D167" t="n">
-        <v>7.1103638060497165E-6</v>
+        <v>7.30370196938962E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>